<commit_message>
student crud routes added
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ibrahim/Documents/python_project/db_system/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59116229-5F2A-4349-ACDC-0EF66CFE297A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4340210E-9E12-9C44-A715-2BFEAD8B358C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16520" xr2:uid="{519AA96D-D64B-C848-85D8-98116B17AEBE}"/>
   </bookViews>
@@ -1122,8 +1122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8650A0-ED64-5B4B-A401-C81B8C806AFE}">
   <dimension ref="A1:Z42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1948,5 +1948,6 @@
     <mergeCell ref="Q2:R2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Institute Income and Expense Form designed
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ibrahim/Documents/python_project/db_system/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4340210E-9E12-9C44-A715-2BFEAD8B358C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E43FAD5-3F33-654F-BB36-DA1B7223297C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16520" xr2:uid="{519AA96D-D64B-C848-85D8-98116B17AEBE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="88">
   <si>
     <t>student_id</t>
   </si>
@@ -269,15 +269,9 @@
     <t>paid_salary</t>
   </si>
   <si>
-    <t>due_salary</t>
-  </si>
-  <si>
     <t>total_fee</t>
   </si>
   <si>
-    <t>due_fee</t>
-  </si>
-  <si>
     <t>instt_income</t>
   </si>
   <si>
@@ -303,6 +297,9 @@
   </si>
   <si>
     <t>Fee</t>
+  </si>
+  <si>
+    <t>day</t>
   </si>
 </sst>
 </file>
@@ -695,7 +692,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -714,6 +711,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -729,61 +762,29 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1120,10 +1121,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8650A0-ED64-5B4B-A401-C81B8C806AFE}">
-  <dimension ref="A1:Z42"/>
+  <dimension ref="A1:Z45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1136,7 +1137,7 @@
     <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.83203125" bestFit="1" customWidth="1"/>
@@ -1151,31 +1152,31 @@
   <sheetData>
     <row r="1" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="27"/>
-      <c r="Q2" s="26" t="s">
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="21"/>
+      <c r="Q2" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="R2" s="27"/>
-      <c r="T2" s="21" t="s">
+      <c r="R2" s="21"/>
+      <c r="T2" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="U2" s="22"/>
+      <c r="U2" s="34"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
@@ -1296,40 +1297,40 @@
     </row>
     <row r="6" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="33"/>
-      <c r="J7" s="26" t="s">
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="19"/>
+      <c r="J7" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="K7" s="27"/>
-      <c r="M7" s="32" t="s">
+      <c r="K7" s="21"/>
+      <c r="M7" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="N7" s="33"/>
-      <c r="P7" s="34" t="s">
+      <c r="N7" s="19"/>
+      <c r="P7" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="Q7" s="35"/>
-      <c r="S7" s="32" t="s">
+      <c r="Q7" s="23"/>
+      <c r="S7" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="T7" s="33"/>
-      <c r="V7" s="32" t="s">
+      <c r="T7" s="19"/>
+      <c r="V7" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="W7" s="33"/>
-      <c r="Y7" s="32" t="s">
+      <c r="W7" s="19"/>
+      <c r="Y7" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="Z7" s="33"/>
+      <c r="Z7" s="19"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
@@ -1354,7 +1355,7 @@
         <v>58</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J8" s="7" t="s">
         <v>57</v>
@@ -1509,66 +1510,78 @@
     </row>
     <row r="13" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="B14" s="36"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="36"/>
-      <c r="J14" s="36"/>
-      <c r="K14" s="36"/>
-      <c r="L14" s="33"/>
-      <c r="O14" s="26" t="s">
+      <c r="A14" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="24"/>
+      <c r="M14" s="24"/>
+      <c r="N14" s="24"/>
+      <c r="O14" s="19"/>
+      <c r="S14" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="P14" s="27"/>
+      <c r="T14" s="21"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
         <v>41</v>
       </c>
       <c r="B15" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="E15" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="F15" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="G15" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="H15" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="13" t="s">
+      <c r="I15" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G15" s="13" t="s">
+      <c r="J15" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="H15" s="13" t="s">
+      <c r="K15" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="I15" s="13" t="s">
+      <c r="L15" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="J15" s="13" t="s">
+      <c r="M15" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="K15" s="13" t="s">
+      <c r="N15" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="L15" s="11" t="s">
+      <c r="O15" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="O15" s="7" t="s">
+      <c r="S15" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="P15" s="9" t="s">
+      <c r="T15" s="9" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1584,11 +1597,14 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
-      <c r="L16" s="3"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="3"/>
-    </row>
-    <row r="17" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="3"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="3"/>
+    </row>
+    <row r="17" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -1600,50 +1616,65 @@
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
-      <c r="L17" s="6"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="6"/>
-    </row>
-    <row r="21" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L22" s="23" t="s">
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="6"/>
+      <c r="S17" s="4"/>
+      <c r="T17" s="6"/>
+    </row>
+    <row r="21" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L22" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="M22" s="24"/>
-      <c r="N22" s="24"/>
-      <c r="O22" s="24"/>
-      <c r="P22" s="24"/>
-      <c r="Q22" s="25"/>
-    </row>
-    <row r="23" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="39" t="s">
+      <c r="M22" s="38"/>
+      <c r="N22" s="38"/>
+      <c r="O22" s="38"/>
+      <c r="P22" s="38"/>
+      <c r="Q22" s="38"/>
+      <c r="R22" s="38"/>
+      <c r="S22" s="38"/>
+      <c r="T22" s="39"/>
+    </row>
+    <row r="23" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="40"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="41"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="29"/>
       <c r="L23" s="10" t="s">
         <v>47</v>
       </c>
       <c r="M23" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="N23" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="O23" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="P23" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="N23" s="13" t="s">
+      <c r="Q23" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="O23" s="13" t="s">
+      <c r="R23" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="P23" s="13" t="s">
+      <c r="S23" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="Q23" s="11" t="s">
+      <c r="T23" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
         <v>16</v>
       </c>
@@ -1667,48 +1698,57 @@
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
-      <c r="Q24" s="3"/>
-    </row>
-    <row r="25" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="3"/>
+    </row>
+    <row r="25" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="L25" s="4"/>
       <c r="M25" s="5"/>
       <c r="N25" s="5"/>
       <c r="O25" s="5"/>
       <c r="P25" s="5"/>
-      <c r="Q25" s="6"/>
-    </row>
-    <row r="26" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I26" s="37" t="s">
+      <c r="Q25" s="5"/>
+      <c r="R25" s="5"/>
+      <c r="S25" s="5"/>
+      <c r="T25" s="6"/>
+    </row>
+    <row r="26" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I26" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="J26" s="38"/>
-    </row>
-    <row r="27" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="18" t="s">
+      <c r="J26" s="26"/>
+    </row>
+    <row r="27" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="20"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="32"/>
       <c r="I27" s="10" t="s">
         <v>64</v>
       </c>
       <c r="J27" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="L27" s="23" t="s">
+      <c r="L27" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="M27" s="24"/>
-      <c r="N27" s="24"/>
-      <c r="O27" s="24"/>
-      <c r="P27" s="24"/>
-      <c r="Q27" s="25"/>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="M27" s="38"/>
+      <c r="N27" s="38"/>
+      <c r="O27" s="38"/>
+      <c r="P27" s="38"/>
+      <c r="Q27" s="38"/>
+      <c r="R27" s="38"/>
+      <c r="S27" s="38"/>
+      <c r="T27" s="39"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
         <v>16</v>
       </c>
@@ -1728,7 +1768,7 @@
         <v>21</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="3"/>
@@ -1736,22 +1776,31 @@
         <v>70</v>
       </c>
       <c r="M28" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="N28" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="O28" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="P28" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="N28" s="13" t="s">
+      <c r="Q28" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="O28" s="13" t="s">
+      <c r="R28" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="P28" s="13" t="s">
+      <c r="S28" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="Q28" s="11" t="s">
+      <c r="T28" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1766,9 +1815,12 @@
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
-      <c r="Q29" s="3"/>
-    </row>
-    <row r="30" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1"/>
+      <c r="T29" s="3"/>
+    </row>
+    <row r="30" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -1781,52 +1833,84 @@
       <c r="N30" s="5"/>
       <c r="O30" s="5"/>
       <c r="P30" s="5"/>
-      <c r="Q30" s="6"/>
-    </row>
-    <row r="32" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="18" t="s">
+      <c r="Q30" s="5"/>
+      <c r="R30" s="5"/>
+      <c r="S30" s="5"/>
+      <c r="T30" s="6"/>
+    </row>
+    <row r="32" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="O32" s="36"/>
+      <c r="P32" s="36"/>
+      <c r="Q32" s="36"/>
+      <c r="R32" s="36"/>
+    </row>
+    <row r="33" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="19"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="20"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B33" s="31"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="31"/>
+      <c r="H33" s="31"/>
+      <c r="I33" s="31"/>
+      <c r="J33" s="31"/>
+      <c r="K33" s="31"/>
+      <c r="L33" s="31"/>
+      <c r="M33" s="32"/>
+      <c r="O33" s="36"/>
+      <c r="P33" s="36"/>
+      <c r="Q33" s="36"/>
+      <c r="R33" s="36"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
         <v>41</v>
       </c>
       <c r="B34" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F34" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="G34" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D34" s="13" t="s">
+      <c r="H34" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E34" s="13" t="s">
+      <c r="I34" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="F34" s="13" t="s">
+      <c r="J34" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="G34" s="13" t="s">
+      <c r="K34" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="H34" s="13" t="s">
+      <c r="L34" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="I34" s="11" t="s">
+      <c r="M34" s="11" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="O34" s="36"/>
+      <c r="P34" s="36"/>
+      <c r="Q34" s="36"/>
+      <c r="R34" s="36"/>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1835,9 +1919,17 @@
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
-      <c r="I35" s="3"/>
-    </row>
-    <row r="36" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="3"/>
+      <c r="O35" s="36"/>
+      <c r="P35" s="36"/>
+      <c r="Q35" s="36"/>
+      <c r="R35" s="36"/>
+    </row>
+    <row r="36" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -1846,60 +1938,83 @@
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
-      <c r="I36" s="6"/>
-    </row>
-    <row r="38" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="28" t="s">
-        <v>85</v>
-      </c>
-      <c r="B39" s="29"/>
-      <c r="C39" s="29"/>
-      <c r="D39" s="29"/>
-      <c r="E39" s="29"/>
-      <c r="F39" s="29"/>
-      <c r="G39" s="29"/>
-      <c r="H39" s="29"/>
-      <c r="I39" s="29"/>
-      <c r="J39" s="29"/>
-      <c r="K39" s="30"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A40" s="7" t="s">
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="6"/>
+    </row>
+    <row r="38" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="36"/>
+      <c r="B38" s="36"/>
+      <c r="C38" s="36"/>
+      <c r="D38" s="36"/>
+      <c r="E38" s="36"/>
+      <c r="F38" s="36"/>
+      <c r="G38" s="36"/>
+      <c r="H38" s="36"/>
+      <c r="I38" s="36"/>
+      <c r="J38" s="36"/>
+      <c r="K38" s="40"/>
+      <c r="L38" s="40"/>
+      <c r="M38" s="41"/>
+      <c r="N38" s="41"/>
+    </row>
+    <row r="39" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="B39" s="44"/>
+      <c r="C39" s="44"/>
+      <c r="D39" s="44"/>
+      <c r="E39" s="44"/>
+      <c r="F39" s="44"/>
+      <c r="G39" s="44"/>
+      <c r="H39" s="44"/>
+      <c r="I39" s="44"/>
+      <c r="J39" s="45"/>
+      <c r="K39" s="42"/>
+      <c r="L39" s="42"/>
+      <c r="M39" s="41"/>
+      <c r="N39" s="41"/>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A40" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B40" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="C40" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D40" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="E40" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F40" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="G40" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="E40" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="F40" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="G40" s="8" t="s">
+      <c r="H40" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="H40" s="8" t="s">
+      <c r="I40" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="I40" s="8" t="s">
+      <c r="J40" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="J40" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="K40" s="9" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K40" s="40"/>
+      <c r="L40" s="40"/>
+      <c r="M40" s="41"/>
+      <c r="N40" s="41"/>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1909,10 +2024,13 @@
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="3"/>
-    </row>
-    <row r="42" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J41" s="3"/>
+      <c r="K41" s="40"/>
+      <c r="L41" s="40"/>
+      <c r="M41" s="41"/>
+      <c r="N41" s="41"/>
+    </row>
+    <row r="42" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
@@ -1922,30 +2040,71 @@
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
-      <c r="J42" s="5"/>
-      <c r="K42" s="6"/>
+      <c r="J42" s="6"/>
+      <c r="K42" s="40"/>
+      <c r="L42" s="40"/>
+      <c r="M42" s="41"/>
+      <c r="N42" s="41"/>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A43" s="36"/>
+      <c r="B43" s="36"/>
+      <c r="C43" s="36"/>
+      <c r="D43" s="36"/>
+      <c r="E43" s="36"/>
+      <c r="F43" s="36"/>
+      <c r="G43" s="36"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="36"/>
+      <c r="K43" s="40"/>
+      <c r="L43" s="40"/>
+      <c r="M43" s="41"/>
+      <c r="N43" s="41"/>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
+      <c r="C44" s="36"/>
+      <c r="D44" s="36"/>
+      <c r="E44" s="36"/>
+      <c r="F44" s="36"/>
+      <c r="G44" s="36"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
+      <c r="K44" s="40"/>
+      <c r="L44" s="40"/>
+      <c r="M44" s="41"/>
+      <c r="N44" s="41"/>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="K45" s="41"/>
+      <c r="L45" s="41"/>
+      <c r="M45" s="41"/>
+      <c r="N45" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="S14:T14"/>
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="A33:M33"/>
+    <mergeCell ref="A14:O14"/>
+    <mergeCell ref="L22:T22"/>
+    <mergeCell ref="L27:T27"/>
+    <mergeCell ref="A39:J39"/>
     <mergeCell ref="Y7:Z7"/>
     <mergeCell ref="M7:N7"/>
     <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L27:Q27"/>
     <mergeCell ref="P7:Q7"/>
     <mergeCell ref="S7:T7"/>
-    <mergeCell ref="A14:L14"/>
     <mergeCell ref="I26:J26"/>
     <mergeCell ref="A23:F23"/>
     <mergeCell ref="A7:H7"/>
     <mergeCell ref="A27:G27"/>
     <mergeCell ref="V7:W7"/>
-    <mergeCell ref="A33:I33"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="L22:Q22"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="A39:K39"/>
-    <mergeCell ref="A2:O2"/>
-    <mergeCell ref="Q2:R2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
orm for fee and salary, account updated
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ibrahim/Documents/python_project/db_system/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70CBFB2F-FF51-FB49-BE35-EA3786E543AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650FC5F3-3C6F-5247-A0C8-F70F874087EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16520" xr2:uid="{519AA96D-D64B-C848-85D8-98116B17AEBE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="97">
   <si>
     <t>student_id</t>
   </si>
@@ -300,6 +300,33 @@
   </si>
   <si>
     <t>day</t>
+  </si>
+  <si>
+    <t>recipt_id</t>
+  </si>
+  <si>
+    <t>total_paid</t>
+  </si>
+  <si>
+    <t>left</t>
+  </si>
+  <si>
+    <t>total_discount</t>
+  </si>
+  <si>
+    <t>Fee_Recipt</t>
+  </si>
+  <si>
+    <t>Teacher_Recipt</t>
+  </si>
+  <si>
+    <t>total_deduction</t>
+  </si>
+  <si>
+    <t>Institute_Recipt</t>
+  </si>
+  <si>
+    <t>record_id</t>
   </si>
 </sst>
 </file>
@@ -354,7 +381,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -638,15 +665,6 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -708,43 +726,64 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -754,38 +793,17 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1122,14 +1140,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8650A0-ED64-5B4B-A401-C81B8C806AFE}">
   <dimension ref="A1:Z52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
@@ -1154,28 +1172,28 @@
       <c r="A2" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
       <c r="O2" s="22"/>
       <c r="Q2" s="21" t="s">
         <v>34</v>
       </c>
       <c r="R2" s="22"/>
-      <c r="T2" s="19" t="s">
+      <c r="T2" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="U2" s="20"/>
+      <c r="U2" s="35"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
@@ -1296,40 +1314,40 @@
     </row>
     <row r="6" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="29"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="20"/>
       <c r="J7" s="21" t="s">
         <v>62</v>
       </c>
       <c r="K7" s="22"/>
-      <c r="M7" s="27" t="s">
+      <c r="M7" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="N7" s="29"/>
-      <c r="P7" s="36" t="s">
+      <c r="N7" s="20"/>
+      <c r="P7" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="Q7" s="37"/>
-      <c r="S7" s="27" t="s">
+      <c r="Q7" s="24"/>
+      <c r="S7" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="T7" s="29"/>
-      <c r="V7" s="27" t="s">
+      <c r="T7" s="20"/>
+      <c r="V7" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="W7" s="29"/>
-      <c r="Y7" s="27" t="s">
+      <c r="W7" s="20"/>
+      <c r="Y7" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="Z7" s="29"/>
+      <c r="Z7" s="20"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
@@ -1509,23 +1527,23 @@
     </row>
     <row r="13" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="28"/>
-      <c r="L14" s="28"/>
-      <c r="M14" s="28"/>
-      <c r="N14" s="28"/>
-      <c r="O14" s="29"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="20"/>
       <c r="S14" s="21" t="s">
         <v>53</v>
       </c>
@@ -1622,414 +1640,455 @@
       <c r="S17" s="4"/>
       <c r="T17" s="6"/>
     </row>
-    <row r="21" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L22" s="30" t="s">
+    <row r="19" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="B20" s="36"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="22"/>
+      <c r="L20" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="M22" s="31"/>
-      <c r="N22" s="31"/>
-      <c r="O22" s="31"/>
-      <c r="P22" s="31"/>
-      <c r="Q22" s="31"/>
-      <c r="R22" s="31"/>
-      <c r="S22" s="31"/>
-      <c r="T22" s="32"/>
+      <c r="M20" s="38"/>
+      <c r="N20" s="38"/>
+      <c r="O20" s="38"/>
+      <c r="P20" s="38"/>
+      <c r="Q20" s="38"/>
+      <c r="R20" s="38"/>
+      <c r="S20" s="38"/>
+      <c r="T20" s="39"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="L21" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="M21" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="N21" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="O21" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="P21" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q21" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="R21" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="S21" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="T21" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A22" s="2"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="3"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="3"/>
     </row>
     <row r="23" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="40" t="s">
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="6"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="5"/>
+      <c r="R23" s="5"/>
+      <c r="S23" s="5"/>
+      <c r="T23" s="6"/>
+    </row>
+    <row r="24" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L25" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="M25" s="38"/>
+      <c r="N25" s="38"/>
+      <c r="O25" s="38"/>
+      <c r="P25" s="38"/>
+      <c r="Q25" s="38"/>
+      <c r="R25" s="38"/>
+      <c r="S25" s="38"/>
+      <c r="T25" s="39"/>
+    </row>
+    <row r="26" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="41"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="42"/>
-      <c r="L23" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="M23" s="13" t="s">
+      <c r="B26" s="28"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="29"/>
+      <c r="L26" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="M26" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="N23" s="13" t="s">
+      <c r="N26" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="O23" s="13" t="s">
+      <c r="O26" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="P23" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q23" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="R23" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="S23" s="13" t="s">
+      <c r="P26" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q26" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="R26" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="S26" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="T23" s="11" t="s">
+      <c r="T26" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
+    <row r="27" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B27" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C27" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="16" t="s">
+      <c r="D27" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E24" s="16" t="s">
+      <c r="E27" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F24" s="17" t="s">
+      <c r="F27" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="L24" s="2"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
-      <c r="Q24" s="1"/>
-      <c r="R24" s="1"/>
-      <c r="S24" s="1"/>
-      <c r="T24" s="3"/>
-    </row>
-    <row r="25" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L25" s="4"/>
-      <c r="M25" s="5"/>
-      <c r="N25" s="5"/>
-      <c r="O25" s="5"/>
-      <c r="P25" s="5"/>
-      <c r="Q25" s="5"/>
-      <c r="R25" s="5"/>
-      <c r="S25" s="5"/>
-      <c r="T25" s="6"/>
-    </row>
-    <row r="26" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I26" s="38" t="s">
+      <c r="L27" s="2"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="3"/>
+    </row>
+    <row r="28" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L28" s="4"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
+      <c r="P28" s="5"/>
+      <c r="Q28" s="5"/>
+      <c r="R28" s="5"/>
+      <c r="S28" s="5"/>
+      <c r="T28" s="6"/>
+    </row>
+    <row r="29" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I29" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="J26" s="39"/>
-    </row>
-    <row r="27" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="24" t="s">
+      <c r="J29" s="26"/>
+    </row>
+    <row r="30" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="26"/>
-      <c r="I27" s="10" t="s">
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="33"/>
+      <c r="I30" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="J27" s="11" t="s">
+      <c r="J30" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="L27" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="M27" s="31"/>
-      <c r="N27" s="31"/>
-      <c r="O27" s="31"/>
-      <c r="P27" s="31"/>
-      <c r="Q27" s="31"/>
-      <c r="R27" s="31"/>
-      <c r="S27" s="31"/>
-      <c r="T27" s="32"/>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A28" s="10" t="s">
+      <c r="L30" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="M30" s="38"/>
+      <c r="N30" s="38"/>
+      <c r="O30" s="39"/>
+      <c r="P30" s="44"/>
+      <c r="Q30" s="44"/>
+      <c r="R30" s="44"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A31" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B31" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C31" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D28" s="13" t="s">
+      <c r="D31" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="E28" s="13" t="s">
+      <c r="E31" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="F28" s="13" t="s">
+      <c r="F31" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="G28" s="11" t="s">
+      <c r="G31" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="I28" s="2"/>
-      <c r="J28" s="3"/>
-      <c r="L28" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="M28" s="13" t="s">
+      <c r="I31" s="2"/>
+      <c r="J31" s="3"/>
+      <c r="L31" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="M31" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="N31" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="O31" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="P31" s="43"/>
+      <c r="Q31" s="43"/>
+      <c r="R31" s="43"/>
+    </row>
+    <row r="32" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="3"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="6"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="3"/>
+      <c r="P32" s="43"/>
+      <c r="Q32" s="43"/>
+      <c r="R32" s="43"/>
+    </row>
+    <row r="33" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="6"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="5"/>
+      <c r="O33" s="6"/>
+      <c r="P33" s="43"/>
+      <c r="Q33" s="43"/>
+      <c r="R33" s="43"/>
+    </row>
+    <row r="35" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" s="32"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="32"/>
+      <c r="G36" s="32"/>
+      <c r="H36" s="32"/>
+      <c r="I36" s="32"/>
+      <c r="J36" s="32"/>
+      <c r="K36" s="32"/>
+      <c r="L36" s="32"/>
+      <c r="M36" s="33"/>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A37" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="N28" s="13" t="s">
+      <c r="C37" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="O28" s="13" t="s">
+      <c r="D37" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="P28" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q28" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="R28" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="S28" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="T28" s="11" t="s">
+      <c r="E37" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F37" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G37" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H37" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="I37" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="J37" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="K37" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="L37" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="M37" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="3"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="6"/>
-      <c r="L29" s="2"/>
-      <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
-      <c r="P29" s="1"/>
-      <c r="Q29" s="1"/>
-      <c r="R29" s="1"/>
-      <c r="S29" s="1"/>
-      <c r="T29" s="3"/>
-    </row>
-    <row r="30" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="6"/>
-      <c r="L30" s="4"/>
-      <c r="M30" s="5"/>
-      <c r="N30" s="5"/>
-      <c r="O30" s="5"/>
-      <c r="P30" s="5"/>
-      <c r="Q30" s="5"/>
-      <c r="R30" s="5"/>
-      <c r="S30" s="5"/>
-      <c r="T30" s="6"/>
-    </row>
-    <row r="32" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="B33" s="25"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
-      <c r="H33" s="25"/>
-      <c r="I33" s="25"/>
-      <c r="J33" s="25"/>
-      <c r="K33" s="25"/>
-      <c r="L33" s="25"/>
-      <c r="M33" s="26"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A34" s="10" t="s">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A38" s="2"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="3"/>
+    </row>
+    <row r="39" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="5"/>
+      <c r="M39" s="6"/>
+    </row>
+    <row r="41" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="B42" s="28"/>
+      <c r="C42" s="28"/>
+      <c r="D42" s="28"/>
+      <c r="E42" s="28"/>
+      <c r="F42" s="28"/>
+      <c r="G42" s="29"/>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A43" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B43" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B34" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="D34" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="E34" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F34" s="13" t="s">
+      <c r="C43" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G34" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="H34" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="I34" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="J34" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="K34" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="L34" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="M34" s="11" t="s">
+      <c r="D43" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G43" s="9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" s="2"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
-      <c r="M35" s="3"/>
-    </row>
-    <row r="36" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="5"/>
-      <c r="J36" s="5"/>
-      <c r="K36" s="5"/>
-      <c r="L36" s="5"/>
-      <c r="M36" s="6"/>
-    </row>
-    <row r="38" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="33" t="s">
-        <v>83</v>
-      </c>
-      <c r="B39" s="34"/>
-      <c r="C39" s="34"/>
-      <c r="D39" s="34"/>
-      <c r="E39" s="34"/>
-      <c r="F39" s="34"/>
-      <c r="G39" s="34"/>
-      <c r="H39" s="34"/>
-      <c r="I39" s="34"/>
-      <c r="J39" s="35"/>
-      <c r="K39" s="18"/>
-      <c r="L39" s="18"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A40" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="B40" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C40" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="D40" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="E40" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="F40" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="G40" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="H40" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="I40" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="J40" s="11" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A41" s="2"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="3"/>
-    </row>
-    <row r="42" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="4"/>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
-      <c r="H42" s="5"/>
-      <c r="I42" s="5"/>
-      <c r="J42" s="6"/>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A44" s="43"/>
-      <c r="B44" s="43"/>
-      <c r="C44" s="43"/>
-      <c r="D44" s="43"/>
-      <c r="E44" s="43"/>
-      <c r="F44" s="43"/>
-      <c r="G44" s="43"/>
-      <c r="H44" s="43"/>
-      <c r="I44" s="43"/>
-      <c r="J44" s="43"/>
-      <c r="K44" s="43"/>
-      <c r="L44" s="43"/>
-      <c r="M44" s="43"/>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A45" s="43"/>
-      <c r="B45" s="43"/>
-      <c r="C45" s="43"/>
-      <c r="D45" s="44"/>
-      <c r="E45" s="44"/>
-      <c r="F45" s="44"/>
-      <c r="G45" s="44"/>
-      <c r="H45" s="44"/>
-      <c r="I45" s="44"/>
-      <c r="J45" s="43"/>
-      <c r="K45" s="43"/>
-      <c r="L45" s="43"/>
-      <c r="M45" s="43"/>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A44" s="2"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="3"/>
+    </row>
+    <row r="45" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="6"/>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46" s="43"/>
       <c r="B46" s="43"/>
       <c r="C46" s="43"/>
@@ -2037,14 +2096,8 @@
       <c r="E46" s="43"/>
       <c r="F46" s="43"/>
       <c r="G46" s="43"/>
-      <c r="H46" s="43"/>
-      <c r="I46" s="43"/>
-      <c r="J46" s="43"/>
-      <c r="K46" s="43"/>
-      <c r="L46" s="43"/>
-      <c r="M46" s="43"/>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A47" s="43"/>
       <c r="B47" s="43"/>
       <c r="C47" s="43"/>
@@ -2052,109 +2105,104 @@
       <c r="E47" s="43"/>
       <c r="F47" s="43"/>
       <c r="G47" s="43"/>
-      <c r="H47" s="43"/>
-      <c r="I47" s="43"/>
-      <c r="J47" s="43"/>
-      <c r="K47" s="43"/>
-      <c r="L47" s="43"/>
-      <c r="M47" s="43"/>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A48" s="43"/>
-      <c r="B48" s="43"/>
-      <c r="C48" s="43"/>
-      <c r="D48" s="43"/>
-      <c r="E48" s="43"/>
-      <c r="F48" s="43"/>
-      <c r="G48" s="43"/>
-      <c r="H48" s="43"/>
-      <c r="I48" s="43"/>
-      <c r="J48" s="43"/>
-      <c r="K48" s="43"/>
-      <c r="L48" s="43"/>
-      <c r="M48" s="43"/>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A49" s="43"/>
-      <c r="B49" s="43"/>
-      <c r="C49" s="43"/>
-      <c r="D49" s="43"/>
-      <c r="E49" s="43"/>
-      <c r="F49" s="43"/>
-      <c r="G49" s="43"/>
-      <c r="H49" s="43"/>
-      <c r="I49" s="43"/>
-      <c r="J49" s="43"/>
-      <c r="K49" s="43"/>
-      <c r="L49" s="43"/>
-      <c r="M49" s="43"/>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A50" s="43"/>
-      <c r="B50" s="43"/>
-      <c r="C50" s="43"/>
-      <c r="D50" s="43"/>
-      <c r="E50" s="43"/>
-      <c r="F50" s="43"/>
-      <c r="G50" s="43"/>
-      <c r="H50" s="43"/>
-      <c r="I50" s="43"/>
-      <c r="J50" s="43"/>
-      <c r="K50" s="43"/>
-      <c r="L50" s="43"/>
-      <c r="M50" s="43"/>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A51" s="43"/>
-      <c r="B51" s="43"/>
-      <c r="C51" s="43"/>
-      <c r="D51" s="43"/>
-      <c r="E51" s="43"/>
-      <c r="F51" s="43"/>
-      <c r="G51" s="43"/>
-      <c r="H51" s="43"/>
-      <c r="I51" s="43"/>
-      <c r="J51" s="43"/>
-      <c r="K51" s="43"/>
-      <c r="L51" s="43"/>
-      <c r="M51" s="43"/>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A52" s="43"/>
-      <c r="B52" s="43"/>
-      <c r="C52" s="43"/>
-      <c r="D52" s="43"/>
-      <c r="E52" s="43"/>
-      <c r="F52" s="43"/>
-      <c r="G52" s="43"/>
-      <c r="H52" s="43"/>
-      <c r="I52" s="43"/>
-      <c r="J52" s="43"/>
-      <c r="K52" s="43"/>
-      <c r="L52" s="43"/>
-      <c r="M52" s="43"/>
+    </row>
+    <row r="48" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="49" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="B49" s="41"/>
+      <c r="C49" s="41"/>
+      <c r="D49" s="41"/>
+      <c r="E49" s="41"/>
+      <c r="F49" s="41"/>
+      <c r="G49" s="41"/>
+      <c r="H49" s="41"/>
+      <c r="I49" s="41"/>
+      <c r="J49" s="42"/>
+      <c r="K49" s="18"/>
+      <c r="L49" s="18"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A50" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B50" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C50" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D50" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="E50" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F50" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="G50" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="H50" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="I50" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="J50" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A51" s="2"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="3"/>
+    </row>
+    <row r="52" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="4"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="5"/>
+      <c r="I52" s="5"/>
+      <c r="J52" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="A39:J39"/>
+  <mergeCells count="22">
+    <mergeCell ref="A42:G42"/>
+    <mergeCell ref="L30:O30"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="S14:T14"/>
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="A36:M36"/>
+    <mergeCell ref="A14:O14"/>
+    <mergeCell ref="L20:T20"/>
+    <mergeCell ref="L25:T25"/>
+    <mergeCell ref="A20:G20"/>
+    <mergeCell ref="A49:J49"/>
     <mergeCell ref="Y7:Z7"/>
     <mergeCell ref="M7:N7"/>
     <mergeCell ref="J7:K7"/>
     <mergeCell ref="P7:Q7"/>
     <mergeCell ref="S7:T7"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="A26:F26"/>
     <mergeCell ref="A7:H7"/>
-    <mergeCell ref="A27:G27"/>
+    <mergeCell ref="A30:G30"/>
     <mergeCell ref="V7:W7"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="S14:T14"/>
-    <mergeCell ref="A2:O2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="A33:M33"/>
-    <mergeCell ref="A14:O14"/>
-    <mergeCell ref="L22:T22"/>
-    <mergeCell ref="L27:T27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Fee form and tables added
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ibrahim/Documents/python_project/db_system/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650FC5F3-3C6F-5247-A0C8-F70F874087EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E8D791-1A6F-CB44-B2CD-0DE02FAC2DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16520" xr2:uid="{519AA96D-D64B-C848-85D8-98116B17AEBE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="94">
   <si>
     <t>student_id</t>
   </si>
@@ -104,9 +104,6 @@
     <t>shift_id</t>
   </si>
   <si>
-    <t>cource_id</t>
-  </si>
-  <si>
     <t>course_id</t>
   </si>
   <si>
@@ -194,12 +191,6 @@
     <t>amount</t>
   </si>
   <si>
-    <t>payment_type_id</t>
-  </si>
-  <si>
-    <t>Payment Type</t>
-  </si>
-  <si>
     <t>Short Course</t>
   </si>
   <si>
@@ -326,7 +317,7 @@
     <t>Institute_Recipt</t>
   </si>
   <si>
-    <t>record_id</t>
+    <t>Expense_Recipt</t>
   </si>
 </sst>
 </file>
@@ -710,7 +701,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -730,16 +721,64 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -754,55 +793,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1140,8 +1134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8650A0-ED64-5B4B-A401-C81B8C806AFE}">
   <dimension ref="A1:Z52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1169,31 +1163,31 @@
   <sheetData>
     <row r="1" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36"/>
-      <c r="O2" s="22"/>
-      <c r="Q2" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="R2" s="22"/>
-      <c r="T2" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="U2" s="35"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="28"/>
+      <c r="Q2" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="R2" s="28"/>
+      <c r="T2" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="U2" s="26"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
@@ -1245,13 +1239,13 @@
         <v>21</v>
       </c>
       <c r="R3" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T3" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="U3" s="11" t="s">
         <v>43</v>
-      </c>
-      <c r="U3" s="11" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
@@ -1274,13 +1268,13 @@
         <v>1</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="T4" s="2">
         <v>1</v>
       </c>
       <c r="U4" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1303,51 +1297,51 @@
         <v>2</v>
       </c>
       <c r="R5" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="T5" s="4">
         <v>2</v>
       </c>
       <c r="U5" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="20"/>
-      <c r="J7" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="K7" s="22"/>
-      <c r="M7" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="N7" s="20"/>
-      <c r="P7" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q7" s="24"/>
-      <c r="S7" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="T7" s="20"/>
-      <c r="V7" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="W7" s="20"/>
-      <c r="Y7" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="Z7" s="20"/>
+      <c r="A7" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="35"/>
+      <c r="J7" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="K7" s="28"/>
+      <c r="M7" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="N7" s="35"/>
+      <c r="P7" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q7" s="40"/>
+      <c r="S7" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="T7" s="35"/>
+      <c r="V7" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="W7" s="35"/>
+      <c r="Y7" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z7" s="35"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
@@ -1357,58 +1351,58 @@
         <v>20</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>21</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F8" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="M8" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="N8" s="11" t="s">
         <v>57</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="K8" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="M8" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="N8" s="11" t="s">
-        <v>60</v>
       </c>
       <c r="P8" s="2" t="s">
         <v>20</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="S8" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T8" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="V8" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="W8" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="Y8" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Z8" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
@@ -1428,25 +1422,25 @@
         <v>1</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="S9" s="2">
         <v>1</v>
       </c>
       <c r="T9" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V9" s="2">
         <v>1</v>
       </c>
       <c r="W9" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Y9" s="2">
         <v>1</v>
       </c>
       <c r="Z9" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
@@ -1466,25 +1460,25 @@
         <v>2</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S10" s="2">
         <v>2</v>
       </c>
       <c r="T10" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="V10" s="2">
         <v>2</v>
       </c>
       <c r="W10" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Y10" s="2">
         <v>2</v>
       </c>
       <c r="Z10" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1504,63 +1498,68 @@
         <v>3</v>
       </c>
       <c r="Q11" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S11" s="4">
         <v>3</v>
       </c>
       <c r="T11" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="V11" s="4">
         <v>3</v>
       </c>
       <c r="W11" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Y11" s="4">
         <v>3</v>
       </c>
       <c r="Z11" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R13" s="43"/>
+      <c r="S13" s="43"/>
+      <c r="T13" s="43"/>
+      <c r="U13" s="43"/>
+    </row>
     <row r="14" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="B14" s="30"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="30"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="30"/>
-      <c r="N14" s="30"/>
-      <c r="O14" s="20"/>
-      <c r="S14" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="T14" s="22"/>
+      <c r="A14" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" s="34"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="35"/>
+      <c r="O14" s="45"/>
+      <c r="R14" s="43"/>
+      <c r="S14" s="44"/>
+      <c r="T14" s="44"/>
+      <c r="U14" s="43"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E15" s="13" t="s">
         <v>0</v>
@@ -1569,38 +1568,34 @@
         <v>20</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H15" s="13" t="s">
         <v>21</v>
       </c>
       <c r="I15" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="K15" s="13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="L15" s="13" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="M15" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="N15" s="13" t="s">
+      <c r="N15" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="O15" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="S15" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="T15" s="9" t="s">
-        <v>1</v>
-      </c>
+      <c r="O15" s="43"/>
+      <c r="R15" s="43"/>
+      <c r="S15" s="43"/>
+      <c r="T15" s="43"/>
+      <c r="U15" s="43"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
@@ -1616,12 +1611,14 @@
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="3"/>
-      <c r="S16" s="2"/>
-      <c r="T16" s="3"/>
-    </row>
-    <row r="17" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="N16" s="3"/>
+      <c r="O16" s="43"/>
+      <c r="R16" s="43"/>
+      <c r="S16" s="43"/>
+      <c r="T16" s="43"/>
+      <c r="U16" s="43"/>
+    </row>
+    <row r="17" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -1635,85 +1632,93 @@
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="6"/>
-      <c r="S17" s="4"/>
-      <c r="T17" s="6"/>
-    </row>
-    <row r="19" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="B20" s="36"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="22"/>
-      <c r="L20" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="M20" s="38"/>
-      <c r="N20" s="38"/>
-      <c r="O20" s="38"/>
-      <c r="P20" s="38"/>
-      <c r="Q20" s="38"/>
-      <c r="R20" s="38"/>
-      <c r="S20" s="38"/>
-      <c r="T20" s="39"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="N17" s="6"/>
+      <c r="O17" s="43"/>
+      <c r="R17" s="43"/>
+      <c r="S17" s="43"/>
+      <c r="T17" s="43"/>
+      <c r="U17" s="43"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="R18" s="43"/>
+      <c r="S18" s="43"/>
+      <c r="T18" s="43"/>
+      <c r="U18" s="43"/>
+    </row>
+    <row r="19" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="28"/>
+      <c r="L20" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="M20" s="23"/>
+      <c r="N20" s="23"/>
+      <c r="O20" s="23"/>
+      <c r="P20" s="23"/>
+      <c r="Q20" s="23"/>
+      <c r="R20" s="23"/>
+      <c r="S20" s="23"/>
+      <c r="T20" s="24"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L21" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="M21" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="N21" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="O21" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="P21" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="M21" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="N21" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="O21" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="P21" s="13" t="s">
+      <c r="Q21" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="Q21" s="13" t="s">
+      <c r="R21" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="R21" s="13" t="s">
+      <c r="S21" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="S21" s="13" t="s">
-        <v>51</v>
-      </c>
       <c r="T21" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1731,7 +1736,7 @@
       <c r="S22" s="1"/>
       <c r="T22" s="3"/>
     </row>
-    <row r="23" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -1749,58 +1754,58 @@
       <c r="S23" s="5"/>
       <c r="T23" s="6"/>
     </row>
-    <row r="24" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L25" s="37" t="s">
+    <row r="24" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L25" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="M25" s="23"/>
+      <c r="N25" s="23"/>
+      <c r="O25" s="23"/>
+      <c r="P25" s="23"/>
+      <c r="Q25" s="23"/>
+      <c r="R25" s="23"/>
+      <c r="S25" s="23"/>
+      <c r="T25" s="24"/>
+    </row>
+    <row r="26" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="21"/>
+      <c r="L26" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="M26" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="N26" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="O26" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="P26" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q26" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="M25" s="38"/>
-      <c r="N25" s="38"/>
-      <c r="O25" s="38"/>
-      <c r="P25" s="38"/>
-      <c r="Q25" s="38"/>
-      <c r="R25" s="38"/>
-      <c r="S25" s="38"/>
-      <c r="T25" s="39"/>
-    </row>
-    <row r="26" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="B26" s="28"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="29"/>
-      <c r="L26" s="10" t="s">
+      <c r="R26" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="M26" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="N26" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="O26" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="P26" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q26" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="R26" s="13" t="s">
-        <v>73</v>
-      </c>
       <c r="S26" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="T26" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
         <v>16</v>
       </c>
@@ -1829,7 +1834,7 @@
       <c r="S27" s="1"/>
       <c r="T27" s="3"/>
     </row>
-    <row r="28" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="L28" s="4"/>
       <c r="M28" s="5"/>
       <c r="N28" s="5"/>
@@ -1840,39 +1845,43 @@
       <c r="S28" s="5"/>
       <c r="T28" s="6"/>
     </row>
-    <row r="29" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I29" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="J29" s="26"/>
-    </row>
-    <row r="30" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="31" t="s">
+    <row r="29" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I29" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="B30" s="32"/>
-      <c r="C30" s="32"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="32"/>
-      <c r="F30" s="32"/>
-      <c r="G30" s="33"/>
+      <c r="J29" s="42"/>
+    </row>
+    <row r="30" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="32"/>
       <c r="I30" s="10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="J30" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="L30" s="37" t="s">
-        <v>95</v>
-      </c>
-      <c r="M30" s="38"/>
-      <c r="N30" s="38"/>
-      <c r="O30" s="39"/>
-      <c r="P30" s="44"/>
-      <c r="Q30" s="44"/>
-      <c r="R30" s="44"/>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+      <c r="L30" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="M30" s="23"/>
+      <c r="N30" s="23"/>
+      <c r="O30" s="24"/>
+      <c r="P30" s="18"/>
+      <c r="Q30" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="R30" s="23"/>
+      <c r="S30" s="23"/>
+      <c r="T30" s="24"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
         <v>16</v>
       </c>
@@ -1880,39 +1889,48 @@
         <v>20</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F31" s="13" t="s">
         <v>21</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I31" s="2"/>
       <c r="J31" s="3"/>
       <c r="L31" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="M31" s="8" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="N31" s="8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="O31" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="P31" s="43"/>
-      <c r="Q31" s="43"/>
-      <c r="R31" s="43"/>
-    </row>
-    <row r="32" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="Q31" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="R31" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="S31" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="T31" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1926,11 +1944,12 @@
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
       <c r="O32" s="3"/>
-      <c r="P32" s="43"/>
-      <c r="Q32" s="43"/>
-      <c r="R32" s="43"/>
-    </row>
-    <row r="33" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q32" s="2"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="3"/>
+    </row>
+    <row r="33" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -1942,70 +1961,69 @@
       <c r="M33" s="5"/>
       <c r="N33" s="5"/>
       <c r="O33" s="6"/>
-      <c r="P33" s="43"/>
-      <c r="Q33" s="43"/>
-      <c r="R33" s="43"/>
-    </row>
-    <row r="35" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="B36" s="32"/>
-      <c r="C36" s="32"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="32"/>
-      <c r="F36" s="32"/>
-      <c r="G36" s="32"/>
-      <c r="H36" s="32"/>
-      <c r="I36" s="32"/>
-      <c r="J36" s="32"/>
-      <c r="K36" s="32"/>
+      <c r="Q33" s="4"/>
+      <c r="R33" s="5"/>
+      <c r="S33" s="5"/>
+      <c r="T33" s="6"/>
+    </row>
+    <row r="35" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" s="31"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="31"/>
+      <c r="G36" s="31"/>
+      <c r="H36" s="31"/>
+      <c r="I36" s="31"/>
+      <c r="J36" s="31"/>
+      <c r="K36" s="31"/>
       <c r="L36" s="32"/>
-      <c r="M36" s="33"/>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="M36" s="45"/>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E37" s="13" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="F37" s="13" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G37" s="13" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H37" s="13" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="I37" s="13" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="J37" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="K37" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="K37" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="L37" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="M37" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="L37" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="M37" s="43"/>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -2017,10 +2035,10 @@
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
-      <c r="L38" s="1"/>
-      <c r="M38" s="3"/>
-    </row>
-    <row r="39" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L38" s="3"/>
+      <c r="M38" s="43"/>
+    </row>
+    <row r="39" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
@@ -2032,45 +2050,48 @@
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
       <c r="K39" s="5"/>
-      <c r="L39" s="5"/>
-      <c r="M39" s="6"/>
-    </row>
-    <row r="41" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="B42" s="28"/>
-      <c r="C42" s="28"/>
-      <c r="D42" s="28"/>
-      <c r="E42" s="28"/>
-      <c r="F42" s="28"/>
-      <c r="G42" s="29"/>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="L39" s="6"/>
+      <c r="M39" s="43"/>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="M40" s="43"/>
+    </row>
+    <row r="41" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B42" s="20"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="21"/>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>16</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -2079,7 +2100,7 @@
       <c r="F44" s="1"/>
       <c r="G44" s="3"/>
     </row>
-    <row r="45" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
@@ -2088,71 +2109,53 @@
       <c r="F45" s="5"/>
       <c r="G45" s="6"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A46" s="43"/>
-      <c r="B46" s="43"/>
-      <c r="C46" s="43"/>
-      <c r="D46" s="43"/>
-      <c r="E46" s="43"/>
-      <c r="F46" s="43"/>
-      <c r="G46" s="43"/>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A47" s="43"/>
-      <c r="B47" s="43"/>
-      <c r="C47" s="43"/>
-      <c r="D47" s="43"/>
-      <c r="E47" s="43"/>
-      <c r="F47" s="43"/>
-      <c r="G47" s="43"/>
-    </row>
-    <row r="48" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="49" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="40" t="s">
-        <v>83</v>
-      </c>
-      <c r="B49" s="41"/>
-      <c r="C49" s="41"/>
-      <c r="D49" s="41"/>
-      <c r="E49" s="41"/>
-      <c r="F49" s="41"/>
-      <c r="G49" s="41"/>
-      <c r="H49" s="41"/>
-      <c r="I49" s="41"/>
-      <c r="J49" s="42"/>
+      <c r="A49" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="B49" s="37"/>
+      <c r="C49" s="37"/>
+      <c r="D49" s="37"/>
+      <c r="E49" s="37"/>
+      <c r="F49" s="37"/>
+      <c r="G49" s="37"/>
+      <c r="H49" s="37"/>
+      <c r="I49" s="37"/>
+      <c r="J49" s="38"/>
       <c r="K49" s="18"/>
       <c r="L49" s="18"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B50" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C50" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="D50" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="B50" s="13" t="s">
+      <c r="E50" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="F50" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="C50" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="D50" s="13" t="s">
+      <c r="G50" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="H50" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="E50" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="F50" s="13" t="s">
+      <c r="I50" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="G50" s="13" t="s">
+      <c r="J50" s="11" t="s">
         <v>79</v>
-      </c>
-      <c r="H50" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="I50" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="J50" s="11" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
@@ -2180,18 +2183,7 @@
       <c r="J52" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="A42:G42"/>
-    <mergeCell ref="L30:O30"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="S14:T14"/>
-    <mergeCell ref="A2:O2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="A36:M36"/>
-    <mergeCell ref="A14:O14"/>
-    <mergeCell ref="L20:T20"/>
-    <mergeCell ref="L25:T25"/>
-    <mergeCell ref="A20:G20"/>
+  <mergeCells count="23">
     <mergeCell ref="A49:J49"/>
     <mergeCell ref="Y7:Z7"/>
     <mergeCell ref="M7:N7"/>
@@ -2203,6 +2195,18 @@
     <mergeCell ref="A7:H7"/>
     <mergeCell ref="A30:G30"/>
     <mergeCell ref="V7:W7"/>
+    <mergeCell ref="A14:N14"/>
+    <mergeCell ref="A36:L36"/>
+    <mergeCell ref="Q30:T30"/>
+    <mergeCell ref="A42:G42"/>
+    <mergeCell ref="L30:O30"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="S14:T14"/>
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="L20:T20"/>
+    <mergeCell ref="L25:T25"/>
+    <mergeCell ref="A20:G20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
the fee sturecture full completed phase - 1
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ibrahim/Documents/python_project/db_system/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E8D791-1A6F-CB44-B2CD-0DE02FAC2DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DACA4050-298E-9C44-95F2-E0EC01C70BB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16520" xr2:uid="{519AA96D-D64B-C848-85D8-98116B17AEBE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="97">
   <si>
     <t>student_id</t>
   </si>
@@ -318,6 +318,15 @@
   </si>
   <si>
     <t>Expense_Recipt</t>
+  </si>
+  <si>
+    <t>fee_type_id</t>
+  </si>
+  <si>
+    <t>fee_type_name</t>
+  </si>
+  <si>
+    <t>mis</t>
   </si>
 </sst>
 </file>
@@ -701,7 +710,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -721,6 +730,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -730,6 +772,18 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -745,59 +799,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1134,8 +1147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8650A0-ED64-5B4B-A401-C81B8C806AFE}">
   <dimension ref="A1:Z52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1152,42 +1165,47 @@
     <col min="13" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="16" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="15.5" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.5" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="12" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="28"/>
-      <c r="Q2" s="27" t="s">
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="25"/>
+      <c r="Q2" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="R2" s="28"/>
-      <c r="T2" s="25" t="s">
+      <c r="R2" s="25"/>
+      <c r="T2" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="U2" s="26"/>
+      <c r="U2" s="41"/>
+      <c r="W2" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="X2" s="41"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
@@ -1246,6 +1264,12 @@
       </c>
       <c r="U3" s="11" t="s">
         <v>43</v>
+      </c>
+      <c r="W3" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="X3" s="11" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
@@ -1276,6 +1300,12 @@
       <c r="U4" s="12" t="s">
         <v>44</v>
       </c>
+      <c r="W4" s="2">
+        <v>1</v>
+      </c>
+      <c r="X4" s="12" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="5" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
@@ -1305,43 +1335,49 @@
       <c r="U5" s="14" t="s">
         <v>44</v>
       </c>
+      <c r="W5" s="4">
+        <v>2</v>
+      </c>
+      <c r="X5" s="14" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="6" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="35"/>
-      <c r="J7" s="27" t="s">
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="23"/>
+      <c r="J7" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="K7" s="28"/>
-      <c r="M7" s="33" t="s">
+      <c r="K7" s="25"/>
+      <c r="M7" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="N7" s="35"/>
-      <c r="P7" s="39" t="s">
+      <c r="N7" s="23"/>
+      <c r="P7" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="Q7" s="40"/>
-      <c r="S7" s="33" t="s">
+      <c r="Q7" s="27"/>
+      <c r="S7" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="T7" s="35"/>
-      <c r="V7" s="33" t="s">
+      <c r="T7" s="23"/>
+      <c r="V7" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="W7" s="35"/>
-      <c r="Y7" s="33" t="s">
+      <c r="W7" s="23"/>
+      <c r="Y7" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="Z7" s="35"/>
+      <c r="Z7" s="23"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
@@ -1520,82 +1556,70 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="R13" s="43"/>
-      <c r="S13" s="43"/>
-      <c r="T13" s="43"/>
-      <c r="U13" s="43"/>
+      <c r="M13" s="46"/>
+      <c r="N13" s="46"/>
     </row>
     <row r="14" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="33" t="s">
+      <c r="A14" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="B14" s="34"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="34"/>
-      <c r="L14" s="34"/>
-      <c r="M14" s="34"/>
-      <c r="N14" s="35"/>
-      <c r="O14" s="45"/>
-      <c r="R14" s="43"/>
-      <c r="S14" s="44"/>
-      <c r="T14" s="44"/>
-      <c r="U14" s="43"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="33"/>
+      <c r="K14" s="33"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="47"/>
+      <c r="N14" s="47"/>
+      <c r="O14" s="44"/>
+      <c r="S14" s="42"/>
+      <c r="T14" s="42"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
         <v>40</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>71</v>
+        <v>0</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>72</v>
+        <v>20</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>84</v>
+        <v>22</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="I15" s="13" t="s">
-        <v>42</v>
+        <v>55</v>
+      </c>
+      <c r="I15" s="49" t="s">
+        <v>94</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="K15" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="L15" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="M15" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="N15" s="11" t="s">
+      <c r="L15" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="O15" s="43"/>
-      <c r="R15" s="43"/>
-      <c r="S15" s="43"/>
-      <c r="T15" s="43"/>
-      <c r="U15" s="43"/>
+      <c r="M15" s="48"/>
+      <c r="N15" s="48"/>
+      <c r="O15" s="45"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
@@ -1609,16 +1633,12 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="43"/>
-      <c r="R16" s="43"/>
-      <c r="S16" s="43"/>
-      <c r="T16" s="43"/>
-      <c r="U16" s="43"/>
-    </row>
-    <row r="17" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L16" s="3"/>
+      <c r="M16" s="45"/>
+      <c r="N16" s="45"/>
+      <c r="O16" s="45"/>
+    </row>
+    <row r="17" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -1630,45 +1650,35 @@
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="43"/>
-      <c r="R17" s="43"/>
-      <c r="S17" s="43"/>
-      <c r="T17" s="43"/>
-      <c r="U17" s="43"/>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="R18" s="43"/>
-      <c r="S18" s="43"/>
-      <c r="T18" s="43"/>
-      <c r="U18" s="43"/>
-    </row>
-    <row r="19" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="27" t="s">
+      <c r="L17" s="6"/>
+      <c r="M17" s="45"/>
+      <c r="N17" s="45"/>
+      <c r="O17" s="45"/>
+    </row>
+    <row r="19" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="B20" s="29"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="28"/>
-      <c r="L20" s="22" t="s">
+      <c r="B20" s="43"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="25"/>
+      <c r="L20" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="M20" s="23"/>
-      <c r="N20" s="23"/>
-      <c r="O20" s="23"/>
-      <c r="P20" s="23"/>
-      <c r="Q20" s="23"/>
-      <c r="R20" s="23"/>
-      <c r="S20" s="23"/>
-      <c r="T20" s="24"/>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="M20" s="38"/>
+      <c r="N20" s="38"/>
+      <c r="O20" s="38"/>
+      <c r="P20" s="38"/>
+      <c r="Q20" s="38"/>
+      <c r="R20" s="38"/>
+      <c r="S20" s="38"/>
+      <c r="T20" s="39"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>85</v>
       </c>
@@ -1718,7 +1728,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1736,7 +1746,7 @@
       <c r="S22" s="1"/>
       <c r="T22" s="3"/>
     </row>
-    <row r="23" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -1754,29 +1764,29 @@
       <c r="S23" s="5"/>
       <c r="T23" s="6"/>
     </row>
-    <row r="24" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L25" s="22" t="s">
+    <row r="24" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L25" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="M25" s="23"/>
-      <c r="N25" s="23"/>
-      <c r="O25" s="23"/>
-      <c r="P25" s="23"/>
-      <c r="Q25" s="23"/>
-      <c r="R25" s="23"/>
-      <c r="S25" s="23"/>
-      <c r="T25" s="24"/>
-    </row>
-    <row r="26" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="19" t="s">
+      <c r="M25" s="38"/>
+      <c r="N25" s="38"/>
+      <c r="O25" s="38"/>
+      <c r="P25" s="38"/>
+      <c r="Q25" s="38"/>
+      <c r="R25" s="38"/>
+      <c r="S25" s="38"/>
+      <c r="T25" s="39"/>
+    </row>
+    <row r="26" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="21"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="32"/>
       <c r="L26" s="10" t="s">
         <v>67</v>
       </c>
@@ -1805,7 +1815,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
         <v>16</v>
       </c>
@@ -1834,7 +1844,7 @@
       <c r="S27" s="1"/>
       <c r="T27" s="3"/>
     </row>
-    <row r="28" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="L28" s="4"/>
       <c r="M28" s="5"/>
       <c r="N28" s="5"/>
@@ -1845,43 +1855,43 @@
       <c r="S28" s="5"/>
       <c r="T28" s="6"/>
     </row>
-    <row r="29" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I29" s="41" t="s">
+    <row r="29" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I29" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="J29" s="42"/>
-    </row>
-    <row r="30" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="30" t="s">
+      <c r="J29" s="29"/>
+    </row>
+    <row r="30" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="32"/>
+      <c r="B30" s="35"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="36"/>
       <c r="I30" s="10" t="s">
         <v>61</v>
       </c>
       <c r="J30" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="L30" s="22" t="s">
+      <c r="L30" s="37" t="s">
         <v>92</v>
       </c>
-      <c r="M30" s="23"/>
-      <c r="N30" s="23"/>
-      <c r="O30" s="24"/>
+      <c r="M30" s="38"/>
+      <c r="N30" s="38"/>
+      <c r="O30" s="39"/>
       <c r="P30" s="18"/>
-      <c r="Q30" s="22" t="s">
+      <c r="Q30" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="R30" s="23"/>
-      <c r="S30" s="23"/>
-      <c r="T30" s="24"/>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="R30" s="38"/>
+      <c r="S30" s="38"/>
+      <c r="T30" s="39"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
         <v>16</v>
       </c>
@@ -1930,7 +1940,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1968,21 +1978,21 @@
     </row>
     <row r="35" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="30" t="s">
+      <c r="A36" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="31"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="31"/>
-      <c r="F36" s="31"/>
-      <c r="G36" s="31"/>
-      <c r="H36" s="31"/>
-      <c r="I36" s="31"/>
-      <c r="J36" s="31"/>
-      <c r="K36" s="31"/>
-      <c r="L36" s="32"/>
-      <c r="M36" s="45"/>
+      <c r="B36" s="35"/>
+      <c r="C36" s="35"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="35"/>
+      <c r="G36" s="35"/>
+      <c r="H36" s="35"/>
+      <c r="I36" s="35"/>
+      <c r="J36" s="35"/>
+      <c r="K36" s="35"/>
+      <c r="L36" s="36"/>
+      <c r="M36" s="18"/>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="s">
@@ -2021,7 +2031,6 @@
       <c r="L37" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="M37" s="43"/>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
@@ -2036,7 +2045,6 @@
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
       <c r="L38" s="3"/>
-      <c r="M38" s="43"/>
     </row>
     <row r="39" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
@@ -2051,22 +2059,18 @@
       <c r="J39" s="5"/>
       <c r="K39" s="5"/>
       <c r="L39" s="6"/>
-      <c r="M39" s="43"/>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="M40" s="43"/>
     </row>
     <row r="41" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="42" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="19" t="s">
+      <c r="A42" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="B42" s="20"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
-      <c r="G42" s="21"/>
+      <c r="B42" s="31"/>
+      <c r="C42" s="31"/>
+      <c r="D42" s="31"/>
+      <c r="E42" s="31"/>
+      <c r="F42" s="31"/>
+      <c r="G42" s="32"/>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
@@ -2111,18 +2115,18 @@
     </row>
     <row r="48" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="49" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="36" t="s">
+      <c r="A49" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="B49" s="37"/>
-      <c r="C49" s="37"/>
-      <c r="D49" s="37"/>
-      <c r="E49" s="37"/>
-      <c r="F49" s="37"/>
-      <c r="G49" s="37"/>
-      <c r="H49" s="37"/>
-      <c r="I49" s="37"/>
-      <c r="J49" s="38"/>
+      <c r="B49" s="20"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="20"/>
+      <c r="H49" s="20"/>
+      <c r="I49" s="20"/>
+      <c r="J49" s="21"/>
       <c r="K49" s="18"/>
       <c r="L49" s="18"/>
     </row>
@@ -2183,7 +2187,16 @@
       <c r="J52" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
+  <mergeCells count="24">
+    <mergeCell ref="L25:T25"/>
+    <mergeCell ref="A20:G20"/>
+    <mergeCell ref="A14:L14"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="S14:T14"/>
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="L20:T20"/>
     <mergeCell ref="A49:J49"/>
     <mergeCell ref="Y7:Z7"/>
     <mergeCell ref="M7:N7"/>
@@ -2195,18 +2208,10 @@
     <mergeCell ref="A7:H7"/>
     <mergeCell ref="A30:G30"/>
     <mergeCell ref="V7:W7"/>
-    <mergeCell ref="A14:N14"/>
     <mergeCell ref="A36:L36"/>
     <mergeCell ref="Q30:T30"/>
     <mergeCell ref="A42:G42"/>
     <mergeCell ref="L30:O30"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="S14:T14"/>
-    <mergeCell ref="A2:O2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="L20:T20"/>
-    <mergeCell ref="L25:T25"/>
-    <mergeCell ref="A20:G20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
changes made to the teacher_registration_orm; salary_type and semester removed from all the tables
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ibrahim/Documents/python_project/db_system/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DACA4050-298E-9C44-95F2-E0EC01C70BB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D6B4908-8EDD-3D48-ADA6-427DA56A55BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16520" xr2:uid="{519AA96D-D64B-C848-85D8-98116B17AEBE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="97">
   <si>
     <t>student_id</t>
   </si>
@@ -710,7 +710,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -730,6 +730,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -739,18 +775,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -772,9 +796,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -784,33 +805,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1147,8 +1143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8650A0-ED64-5B4B-A401-C81B8C806AFE}">
   <dimension ref="A1:Z52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1177,35 +1173,35 @@
   <sheetData>
     <row r="1" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="43"/>
-      <c r="O2" s="25"/>
-      <c r="Q2" s="24" t="s">
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="24"/>
+      <c r="Q2" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="R2" s="25"/>
-      <c r="T2" s="40" t="s">
+      <c r="R2" s="24"/>
+      <c r="T2" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="U2" s="41"/>
-      <c r="W2" s="40" t="s">
+      <c r="U2" s="29"/>
+      <c r="W2" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="X2" s="41"/>
+      <c r="X2" s="29"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
@@ -1344,40 +1340,40 @@
     </row>
     <row r="6" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="23"/>
-      <c r="J7" s="24" t="s">
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="27"/>
+      <c r="J7" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="K7" s="25"/>
-      <c r="M7" s="22" t="s">
+      <c r="K7" s="24"/>
+      <c r="M7" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="N7" s="23"/>
-      <c r="P7" s="26" t="s">
+      <c r="N7" s="27"/>
+      <c r="P7" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="Q7" s="27"/>
-      <c r="S7" s="22" t="s">
+      <c r="Q7" s="35"/>
+      <c r="S7" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="T7" s="23"/>
-      <c r="V7" s="22" t="s">
+      <c r="T7" s="27"/>
+      <c r="V7" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="W7" s="23"/>
-      <c r="Y7" s="22" t="s">
+      <c r="W7" s="27"/>
+      <c r="Y7" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="Z7" s="23"/>
+      <c r="Z7" s="27"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
@@ -1555,30 +1551,27 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="M13" s="46"/>
-      <c r="N13" s="46"/>
-    </row>
+    <row r="13" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="B14" s="33"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="33"/>
-      <c r="K14" s="33"/>
-      <c r="L14" s="23"/>
-      <c r="M14" s="47"/>
-      <c r="N14" s="47"/>
-      <c r="O14" s="44"/>
-      <c r="S14" s="42"/>
-      <c r="T14" s="42"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="18"/>
+      <c r="S14" s="30"/>
+      <c r="T14" s="30"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
@@ -1605,7 +1598,7 @@
       <c r="H15" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="I15" s="49" t="s">
+      <c r="I15" s="13" t="s">
         <v>94</v>
       </c>
       <c r="J15" s="13" t="s">
@@ -1617,9 +1610,6 @@
       <c r="L15" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="M15" s="48"/>
-      <c r="N15" s="48"/>
-      <c r="O15" s="45"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
@@ -1634,9 +1624,6 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="3"/>
-      <c r="M16" s="45"/>
-      <c r="N16" s="45"/>
-      <c r="O16" s="45"/>
     </row>
     <row r="17" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
@@ -1651,32 +1638,29 @@
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
       <c r="L17" s="6"/>
-      <c r="M17" s="45"/>
-      <c r="N17" s="45"/>
-      <c r="O17" s="45"/>
     </row>
     <row r="19" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="24" t="s">
+      <c r="A20" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="B20" s="43"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="25"/>
-      <c r="L20" s="37" t="s">
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="24"/>
+      <c r="L20" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="M20" s="38"/>
-      <c r="N20" s="38"/>
-      <c r="O20" s="38"/>
-      <c r="P20" s="38"/>
-      <c r="Q20" s="38"/>
-      <c r="R20" s="38"/>
-      <c r="S20" s="38"/>
-      <c r="T20" s="39"/>
+      <c r="M20" s="20"/>
+      <c r="N20" s="20"/>
+      <c r="O20" s="20"/>
+      <c r="P20" s="20"/>
+      <c r="Q20" s="20"/>
+      <c r="R20" s="20"/>
+      <c r="S20" s="20"/>
+      <c r="T20" s="21"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
@@ -1766,27 +1750,27 @@
     </row>
     <row r="24" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L25" s="37" t="s">
+      <c r="L25" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="M25" s="38"/>
-      <c r="N25" s="38"/>
-      <c r="O25" s="38"/>
-      <c r="P25" s="38"/>
-      <c r="Q25" s="38"/>
-      <c r="R25" s="38"/>
-      <c r="S25" s="38"/>
-      <c r="T25" s="39"/>
+      <c r="M25" s="20"/>
+      <c r="N25" s="20"/>
+      <c r="O25" s="20"/>
+      <c r="P25" s="20"/>
+      <c r="Q25" s="20"/>
+      <c r="R25" s="20"/>
+      <c r="S25" s="20"/>
+      <c r="T25" s="21"/>
     </row>
     <row r="26" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="30" t="s">
+      <c r="A26" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="31"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="32"/>
+      <c r="B26" s="39"/>
+      <c r="C26" s="39"/>
+      <c r="D26" s="39"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="40"/>
       <c r="L26" s="10" t="s">
         <v>67</v>
       </c>
@@ -1856,40 +1840,40 @@
       <c r="T28" s="6"/>
     </row>
     <row r="29" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I29" s="28" t="s">
+      <c r="I29" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="J29" s="29"/>
+      <c r="J29" s="37"/>
     </row>
     <row r="30" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="34" t="s">
+      <c r="A30" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="B30" s="35"/>
-      <c r="C30" s="35"/>
-      <c r="D30" s="35"/>
-      <c r="E30" s="35"/>
-      <c r="F30" s="35"/>
-      <c r="G30" s="36"/>
+      <c r="B30" s="42"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="44"/>
+      <c r="G30" s="44"/>
       <c r="I30" s="10" t="s">
         <v>61</v>
       </c>
       <c r="J30" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="L30" s="37" t="s">
+      <c r="L30" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="M30" s="38"/>
-      <c r="N30" s="38"/>
-      <c r="O30" s="39"/>
+      <c r="M30" s="20"/>
+      <c r="N30" s="20"/>
+      <c r="O30" s="21"/>
       <c r="P30" s="18"/>
-      <c r="Q30" s="37" t="s">
+      <c r="Q30" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="R30" s="38"/>
-      <c r="S30" s="38"/>
-      <c r="T30" s="39"/>
+      <c r="R30" s="20"/>
+      <c r="S30" s="20"/>
+      <c r="T30" s="21"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
@@ -1902,17 +1886,13 @@
         <v>22</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="E31" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="F31" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="G31" s="11" t="s">
+      <c r="E31" s="11" t="s">
         <v>82</v>
       </c>
+      <c r="F31" s="45"/>
+      <c r="G31" s="45"/>
       <c r="I31" s="2"/>
       <c r="J31" s="3"/>
       <c r="L31" s="7" t="s">
@@ -1945,9 +1925,9 @@
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="45"/>
+      <c r="G32" s="45"/>
       <c r="I32" s="4"/>
       <c r="J32" s="6"/>
       <c r="L32" s="2"/>
@@ -1964,9 +1944,9 @@
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="45"/>
+      <c r="G33" s="45"/>
       <c r="L33" s="4"/>
       <c r="M33" s="5"/>
       <c r="N33" s="5"/>
@@ -1978,20 +1958,20 @@
     </row>
     <row r="35" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="34" t="s">
+      <c r="A36" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="35"/>
-      <c r="C36" s="35"/>
-      <c r="D36" s="35"/>
-      <c r="E36" s="35"/>
-      <c r="F36" s="35"/>
-      <c r="G36" s="35"/>
-      <c r="H36" s="35"/>
-      <c r="I36" s="35"/>
-      <c r="J36" s="35"/>
-      <c r="K36" s="35"/>
-      <c r="L36" s="36"/>
+      <c r="B36" s="42"/>
+      <c r="C36" s="42"/>
+      <c r="D36" s="42"/>
+      <c r="E36" s="42"/>
+      <c r="F36" s="42"/>
+      <c r="G36" s="42"/>
+      <c r="H36" s="43"/>
+      <c r="I36" s="44"/>
+      <c r="J36" s="44"/>
+      <c r="K36" s="44"/>
+      <c r="L36" s="44"/>
       <c r="M36" s="18"/>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.2">
@@ -1999,38 +1979,30 @@
         <v>40</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>71</v>
+        <v>16</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>72</v>
+        <v>20</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>84</v>
+        <v>22</v>
       </c>
       <c r="E37" s="13" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="F37" s="13" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="G37" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="H37" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="I37" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="J37" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="K37" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="L37" s="11" t="s">
+      <c r="H37" s="11" t="s">
         <v>39</v>
       </c>
+      <c r="I37" s="45"/>
+      <c r="J37" s="45"/>
+      <c r="K37" s="45"/>
+      <c r="L37" s="45"/>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
@@ -2040,11 +2012,11 @@
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
-      <c r="L38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="45"/>
+      <c r="J38" s="45"/>
+      <c r="K38" s="45"/>
+      <c r="L38" s="45"/>
     </row>
     <row r="39" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
@@ -2054,23 +2026,26 @@
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
-      <c r="H39" s="5"/>
-      <c r="I39" s="5"/>
-      <c r="J39" s="5"/>
-      <c r="K39" s="5"/>
-      <c r="L39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="45"/>
+      <c r="J39" s="45"/>
+      <c r="K39" s="45"/>
+      <c r="L39" s="45"/>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="I40" s="45"/>
     </row>
     <row r="41" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="42" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="B42" s="31"/>
-      <c r="C42" s="31"/>
-      <c r="D42" s="31"/>
-      <c r="E42" s="31"/>
-      <c r="F42" s="31"/>
-      <c r="G42" s="32"/>
+      <c r="B42" s="39"/>
+      <c r="C42" s="39"/>
+      <c r="D42" s="39"/>
+      <c r="E42" s="39"/>
+      <c r="F42" s="39"/>
+      <c r="G42" s="40"/>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
@@ -2115,18 +2090,18 @@
     </row>
     <row r="48" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="49" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="19" t="s">
+      <c r="A49" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="B49" s="20"/>
-      <c r="C49" s="20"/>
-      <c r="D49" s="20"/>
-      <c r="E49" s="20"/>
-      <c r="F49" s="20"/>
-      <c r="G49" s="20"/>
-      <c r="H49" s="20"/>
-      <c r="I49" s="20"/>
-      <c r="J49" s="21"/>
+      <c r="B49" s="32"/>
+      <c r="C49" s="32"/>
+      <c r="D49" s="32"/>
+      <c r="E49" s="32"/>
+      <c r="F49" s="32"/>
+      <c r="G49" s="32"/>
+      <c r="H49" s="32"/>
+      <c r="I49" s="32"/>
+      <c r="J49" s="33"/>
       <c r="K49" s="18"/>
       <c r="L49" s="18"/>
     </row>
@@ -2188,6 +2163,21 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A36:H36"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="A49:J49"/>
+    <mergeCell ref="Y7:Z7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="A26:F26"/>
+    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="V7:W7"/>
+    <mergeCell ref="Q30:T30"/>
+    <mergeCell ref="A42:G42"/>
+    <mergeCell ref="L30:O30"/>
     <mergeCell ref="L25:T25"/>
     <mergeCell ref="A20:G20"/>
     <mergeCell ref="A14:L14"/>
@@ -2197,21 +2187,6 @@
     <mergeCell ref="A2:O2"/>
     <mergeCell ref="Q2:R2"/>
     <mergeCell ref="L20:T20"/>
-    <mergeCell ref="A49:J49"/>
-    <mergeCell ref="Y7:Z7"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="S7:T7"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="A26:F26"/>
-    <mergeCell ref="A7:H7"/>
-    <mergeCell ref="A30:G30"/>
-    <mergeCell ref="V7:W7"/>
-    <mergeCell ref="A36:L36"/>
-    <mergeCell ref="Q30:T30"/>
-    <mergeCell ref="A42:G42"/>
-    <mergeCell ref="L30:O30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
COMPLETED THE TEACHER SALARY MODULE
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ibrahim/Documents/python_project/db_system/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D6B4908-8EDD-3D48-ADA6-427DA56A55BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8398B61E-D969-2646-B9F4-7F24B30BD689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16520" xr2:uid="{519AA96D-D64B-C848-85D8-98116B17AEBE}"/>
   </bookViews>
@@ -1143,8 +1143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8650A0-ED64-5B4B-A401-C81B8C806AFE}">
   <dimension ref="A1:Z52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
some updates are made to the previous moduels
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ibrahim/Documents/python_project/db_system/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8398B61E-D969-2646-B9F4-7F24B30BD689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE941828-64DF-C54E-8819-FF8919522D64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16520" xr2:uid="{519AA96D-D64B-C848-85D8-98116B17AEBE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="103">
   <si>
     <t>student_id</t>
   </si>
@@ -327,6 +327,24 @@
   </si>
   <si>
     <t>mis</t>
+  </si>
+  <si>
+    <t>Contract Type</t>
+  </si>
+  <si>
+    <t>contract_type_id</t>
+  </si>
+  <si>
+    <t>contract_type_name</t>
+  </si>
+  <si>
+    <t>Yearly</t>
+  </si>
+  <si>
+    <t>Salary</t>
+  </si>
+  <si>
+    <t>Bonus</t>
   </si>
 </sst>
 </file>
@@ -710,7 +728,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -730,6 +748,60 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -739,24 +811,9 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -766,47 +823,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1143,13 +1159,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8650A0-ED64-5B4B-A401-C81B8C806AFE}">
   <dimension ref="A1:Z52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
@@ -1173,35 +1190,35 @@
   <sheetData>
     <row r="1" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="24"/>
-      <c r="Q2" s="22" t="s">
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="28"/>
+      <c r="Q2" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="R2" s="24"/>
-      <c r="T2" s="28" t="s">
+      <c r="R2" s="28"/>
+      <c r="T2" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="U2" s="29"/>
-      <c r="W2" s="28" t="s">
+      <c r="U2" s="42"/>
+      <c r="W2" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="X2" s="29"/>
+      <c r="X2" s="42"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
@@ -1343,37 +1360,37 @@
       <c r="A7" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="27"/>
-      <c r="J7" s="22" t="s">
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="26"/>
+      <c r="J7" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="K7" s="24"/>
+      <c r="K7" s="28"/>
       <c r="M7" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="N7" s="27"/>
-      <c r="P7" s="34" t="s">
+      <c r="N7" s="26"/>
+      <c r="P7" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="Q7" s="35"/>
+      <c r="Q7" s="30"/>
       <c r="S7" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="T7" s="27"/>
+      <c r="T7" s="26"/>
       <c r="V7" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="W7" s="27"/>
+      <c r="W7" s="26"/>
       <c r="Y7" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="Z7" s="27"/>
+      <c r="Z7" s="26"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
@@ -1556,22 +1573,22 @@
       <c r="A14" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="27"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="36"/>
+      <c r="K14" s="36"/>
+      <c r="L14" s="26"/>
       <c r="M14" s="18"/>
       <c r="N14" s="18"/>
       <c r="O14" s="18"/>
-      <c r="S14" s="30"/>
-      <c r="T14" s="30"/>
+      <c r="S14" s="43"/>
+      <c r="T14" s="43"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
@@ -1641,26 +1658,26 @@
     </row>
     <row r="19" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="24"/>
-      <c r="L20" s="19" t="s">
+      <c r="B20" s="40"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="28"/>
+      <c r="L20" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="M20" s="20"/>
-      <c r="N20" s="20"/>
-      <c r="O20" s="20"/>
-      <c r="P20" s="20"/>
-      <c r="Q20" s="20"/>
-      <c r="R20" s="20"/>
-      <c r="S20" s="20"/>
-      <c r="T20" s="21"/>
+      <c r="M20" s="38"/>
+      <c r="N20" s="38"/>
+      <c r="O20" s="38"/>
+      <c r="P20" s="38"/>
+      <c r="Q20" s="38"/>
+      <c r="R20" s="38"/>
+      <c r="S20" s="38"/>
+      <c r="T20" s="39"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
@@ -1750,27 +1767,27 @@
     </row>
     <row r="24" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L25" s="19" t="s">
+      <c r="L25" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="M25" s="20"/>
-      <c r="N25" s="20"/>
-      <c r="O25" s="20"/>
-      <c r="P25" s="20"/>
-      <c r="Q25" s="20"/>
-      <c r="R25" s="20"/>
-      <c r="S25" s="20"/>
-      <c r="T25" s="21"/>
+      <c r="M25" s="38"/>
+      <c r="N25" s="38"/>
+      <c r="O25" s="38"/>
+      <c r="P25" s="38"/>
+      <c r="Q25" s="38"/>
+      <c r="R25" s="38"/>
+      <c r="S25" s="38"/>
+      <c r="T25" s="39"/>
     </row>
     <row r="26" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="38" t="s">
+      <c r="A26" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="39"/>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="40"/>
+      <c r="B26" s="34"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="35"/>
       <c r="L26" s="10" t="s">
         <v>67</v>
       </c>
@@ -1840,40 +1857,40 @@
       <c r="T28" s="6"/>
     </row>
     <row r="29" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I29" s="36" t="s">
+      <c r="I29" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="J29" s="37"/>
+      <c r="J29" s="32"/>
     </row>
     <row r="30" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="41" t="s">
+      <c r="A30" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="B30" s="42"/>
-      <c r="C30" s="42"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="44"/>
-      <c r="G30" s="44"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
       <c r="I30" s="10" t="s">
         <v>61</v>
       </c>
       <c r="J30" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="L30" s="19" t="s">
+      <c r="L30" s="37" t="s">
         <v>92</v>
       </c>
-      <c r="M30" s="20"/>
-      <c r="N30" s="20"/>
-      <c r="O30" s="21"/>
+      <c r="M30" s="38"/>
+      <c r="N30" s="38"/>
+      <c r="O30" s="39"/>
       <c r="P30" s="18"/>
-      <c r="Q30" s="19" t="s">
+      <c r="Q30" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="R30" s="20"/>
-      <c r="S30" s="20"/>
-      <c r="T30" s="21"/>
+      <c r="R30" s="38"/>
+      <c r="S30" s="38"/>
+      <c r="T30" s="39"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
@@ -1883,7 +1900,7 @@
         <v>20</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>22</v>
+        <v>98</v>
       </c>
       <c r="D31" s="13" t="s">
         <v>21</v>
@@ -1891,10 +1908,12 @@
       <c r="E31" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="F31" s="45"/>
-      <c r="G31" s="45"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="3"/>
+      <c r="I31" s="2">
+        <v>1</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="L31" s="7" t="s">
         <v>85</v>
       </c>
@@ -1926,10 +1945,12 @@
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="3"/>
-      <c r="F32" s="45"/>
-      <c r="G32" s="45"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="6"/>
+      <c r="I32" s="4">
+        <v>2</v>
+      </c>
+      <c r="J32" s="6" t="s">
+        <v>102</v>
+      </c>
       <c r="L32" s="2"/>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
@@ -1945,8 +1966,6 @@
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="6"/>
-      <c r="F33" s="45"/>
-      <c r="G33" s="45"/>
       <c r="L33" s="4"/>
       <c r="M33" s="5"/>
       <c r="N33" s="5"/>
@@ -1958,23 +1977,23 @@
     </row>
     <row r="35" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="41" t="s">
+      <c r="A36" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="42"/>
-      <c r="C36" s="42"/>
-      <c r="D36" s="42"/>
-      <c r="E36" s="42"/>
-      <c r="F36" s="42"/>
-      <c r="G36" s="42"/>
-      <c r="H36" s="43"/>
-      <c r="I36" s="44"/>
-      <c r="J36" s="44"/>
-      <c r="K36" s="44"/>
-      <c r="L36" s="44"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="18"/>
+      <c r="L36" s="18"/>
       <c r="M36" s="18"/>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>40</v>
       </c>
@@ -1985,7 +2004,7 @@
         <v>20</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>22</v>
+        <v>98</v>
       </c>
       <c r="E37" s="13" t="s">
         <v>61</v>
@@ -1999,24 +2018,25 @@
       <c r="H37" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="I37" s="45"/>
-      <c r="J37" s="45"/>
-      <c r="K37" s="45"/>
-      <c r="L37" s="45"/>
+      <c r="J37" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="K37" s="32"/>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="3"/>
-      <c r="I38" s="45"/>
-      <c r="J38" s="45"/>
-      <c r="K38" s="45"/>
-      <c r="L38" s="45"/>
+      <c r="J38" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="K38" s="11" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="39" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
@@ -2027,25 +2047,28 @@
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
       <c r="H39" s="6"/>
-      <c r="I39" s="45"/>
-      <c r="J39" s="45"/>
-      <c r="K39" s="45"/>
-      <c r="L39" s="45"/>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="I40" s="45"/>
+      <c r="J39" s="2">
+        <v>1</v>
+      </c>
+      <c r="K39" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J40" s="4"/>
+      <c r="K40" s="6"/>
     </row>
     <row r="41" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="42" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="38" t="s">
+      <c r="A42" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="B42" s="39"/>
-      <c r="C42" s="39"/>
-      <c r="D42" s="39"/>
-      <c r="E42" s="39"/>
-      <c r="F42" s="39"/>
-      <c r="G42" s="40"/>
+      <c r="B42" s="34"/>
+      <c r="C42" s="34"/>
+      <c r="D42" s="34"/>
+      <c r="E42" s="34"/>
+      <c r="F42" s="34"/>
+      <c r="G42" s="35"/>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
@@ -2090,18 +2113,18 @@
     </row>
     <row r="48" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="49" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="31" t="s">
+      <c r="A49" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="B49" s="32"/>
-      <c r="C49" s="32"/>
-      <c r="D49" s="32"/>
-      <c r="E49" s="32"/>
-      <c r="F49" s="32"/>
-      <c r="G49" s="32"/>
-      <c r="H49" s="32"/>
-      <c r="I49" s="32"/>
-      <c r="J49" s="33"/>
+      <c r="B49" s="23"/>
+      <c r="C49" s="23"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="23"/>
+      <c r="F49" s="23"/>
+      <c r="G49" s="23"/>
+      <c r="H49" s="23"/>
+      <c r="I49" s="23"/>
+      <c r="J49" s="24"/>
       <c r="K49" s="18"/>
       <c r="L49" s="18"/>
     </row>
@@ -2162,7 +2185,16 @@
       <c r="J52" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="25">
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="A20:G20"/>
+    <mergeCell ref="A14:L14"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="S14:T14"/>
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="L20:T20"/>
     <mergeCell ref="A36:H36"/>
     <mergeCell ref="A30:E30"/>
     <mergeCell ref="A49:J49"/>
@@ -2179,14 +2211,6 @@
     <mergeCell ref="A42:G42"/>
     <mergeCell ref="L30:O30"/>
     <mergeCell ref="L25:T25"/>
-    <mergeCell ref="A20:G20"/>
-    <mergeCell ref="A14:L14"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="S14:T14"/>
-    <mergeCell ref="A2:O2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="L20:T20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
doc orm, router and form added
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ibrahim/Documents/python_project/db_system/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A32825-7A31-AD4C-8BA6-ABFF85D7800D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5895898-CE4A-A843-A6F6-826F3B623FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16520" xr2:uid="{519AA96D-D64B-C848-85D8-98116B17AEBE}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15640" xr2:uid="{519AA96D-D64B-C848-85D8-98116B17AEBE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="108">
   <si>
     <t>student_id</t>
   </si>
@@ -345,6 +345,21 @@
   </si>
   <si>
     <t>Bonus</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Recived By</t>
+  </si>
+  <si>
+    <t>Doc Type</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -748,6 +763,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -766,30 +823,12 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -797,30 +836,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1159,8 +1174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8650A0-ED64-5B4B-A401-C81B8C806AFE}">
   <dimension ref="A1:Z52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" topLeftCell="G31" workbookViewId="0">
+      <selection activeCell="Q41" sqref="Q41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1190,35 +1205,35 @@
   <sheetData>
     <row r="1" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="28"/>
-      <c r="Q2" s="27" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="23"/>
+      <c r="Q2" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="R2" s="28"/>
-      <c r="T2" s="41" t="s">
+      <c r="R2" s="23"/>
+      <c r="T2" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="U2" s="42"/>
-      <c r="W2" s="41" t="s">
+      <c r="U2" s="28"/>
+      <c r="W2" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="X2" s="42"/>
+      <c r="X2" s="28"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
@@ -1357,37 +1372,37 @@
     </row>
     <row r="6" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
       <c r="H7" s="26"/>
-      <c r="J7" s="27" t="s">
+      <c r="J7" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="K7" s="28"/>
-      <c r="M7" s="25" t="s">
+      <c r="K7" s="23"/>
+      <c r="M7" s="24" t="s">
         <v>58</v>
       </c>
       <c r="N7" s="26"/>
-      <c r="P7" s="29" t="s">
+      <c r="P7" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="Q7" s="30"/>
-      <c r="S7" s="25" t="s">
+      <c r="Q7" s="40"/>
+      <c r="S7" s="24" t="s">
         <v>52</v>
       </c>
       <c r="T7" s="26"/>
-      <c r="V7" s="25" t="s">
+      <c r="V7" s="24" t="s">
         <v>51</v>
       </c>
       <c r="W7" s="26"/>
-      <c r="Y7" s="25" t="s">
+      <c r="Y7" s="24" t="s">
         <v>53</v>
       </c>
       <c r="Z7" s="26"/>
@@ -1570,25 +1585,25 @@
     </row>
     <row r="13" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="B14" s="36"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="36"/>
-      <c r="J14" s="36"/>
-      <c r="K14" s="36"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
       <c r="L14" s="26"/>
       <c r="M14" s="18"/>
       <c r="N14" s="18"/>
       <c r="O14" s="18"/>
-      <c r="S14" s="43"/>
-      <c r="T14" s="43"/>
+      <c r="S14" s="29"/>
+      <c r="T14" s="29"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
@@ -1658,26 +1673,26 @@
     </row>
     <row r="19" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="B20" s="40"/>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
-      <c r="F20" s="40"/>
-      <c r="G20" s="28"/>
-      <c r="L20" s="37" t="s">
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="23"/>
+      <c r="L20" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="M20" s="38"/>
-      <c r="N20" s="38"/>
-      <c r="O20" s="38"/>
-      <c r="P20" s="38"/>
-      <c r="Q20" s="38"/>
-      <c r="R20" s="38"/>
-      <c r="S20" s="38"/>
-      <c r="T20" s="39"/>
+      <c r="M20" s="31"/>
+      <c r="N20" s="31"/>
+      <c r="O20" s="31"/>
+      <c r="P20" s="31"/>
+      <c r="Q20" s="31"/>
+      <c r="R20" s="31"/>
+      <c r="S20" s="31"/>
+      <c r="T20" s="32"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
@@ -1767,27 +1782,27 @@
     </row>
     <row r="24" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L25" s="37" t="s">
+      <c r="L25" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="M25" s="38"/>
-      <c r="N25" s="38"/>
-      <c r="O25" s="38"/>
-      <c r="P25" s="38"/>
-      <c r="Q25" s="38"/>
-      <c r="R25" s="38"/>
-      <c r="S25" s="38"/>
-      <c r="T25" s="39"/>
+      <c r="M25" s="31"/>
+      <c r="N25" s="31"/>
+      <c r="O25" s="31"/>
+      <c r="P25" s="31"/>
+      <c r="Q25" s="31"/>
+      <c r="R25" s="31"/>
+      <c r="S25" s="31"/>
+      <c r="T25" s="32"/>
     </row>
     <row r="26" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="33" t="s">
+      <c r="A26" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="34"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="35"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="43"/>
       <c r="L26" s="10" t="s">
         <v>67</v>
       </c>
@@ -1857,19 +1872,19 @@
       <c r="T28" s="6"/>
     </row>
     <row r="29" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I29" s="31" t="s">
+      <c r="I29" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="J29" s="32"/>
+      <c r="J29" s="20"/>
     </row>
     <row r="30" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="19" t="s">
+      <c r="A30" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="21"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="34"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="35"/>
       <c r="F30" s="18"/>
       <c r="G30" s="18"/>
       <c r="I30" s="10" t="s">
@@ -1878,19 +1893,19 @@
       <c r="J30" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="L30" s="37" t="s">
+      <c r="L30" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="M30" s="38"/>
-      <c r="N30" s="38"/>
-      <c r="O30" s="39"/>
+      <c r="M30" s="31"/>
+      <c r="N30" s="31"/>
+      <c r="O30" s="32"/>
       <c r="P30" s="18"/>
-      <c r="Q30" s="37" t="s">
+      <c r="Q30" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="R30" s="38"/>
-      <c r="S30" s="38"/>
-      <c r="T30" s="39"/>
+      <c r="R30" s="31"/>
+      <c r="S30" s="31"/>
+      <c r="T30" s="32"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
@@ -1977,16 +1992,16 @@
     </row>
     <row r="35" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="19" t="s">
+      <c r="A36" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="20"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="20"/>
-      <c r="H36" s="21"/>
+      <c r="B36" s="34"/>
+      <c r="C36" s="34"/>
+      <c r="D36" s="34"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
+      <c r="G36" s="34"/>
+      <c r="H36" s="35"/>
       <c r="I36" s="18"/>
       <c r="J36" s="18"/>
       <c r="K36" s="18"/>
@@ -2018,10 +2033,10 @@
       <c r="H37" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="J37" s="31" t="s">
+      <c r="J37" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="K37" s="32"/>
+      <c r="K37" s="20"/>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
@@ -2060,15 +2075,15 @@
     </row>
     <row r="41" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="42" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="33" t="s">
+      <c r="A42" s="41" t="s">
         <v>90</v>
       </c>
-      <c r="B42" s="34"/>
-      <c r="C42" s="34"/>
-      <c r="D42" s="34"/>
-      <c r="E42" s="34"/>
-      <c r="F42" s="34"/>
-      <c r="G42" s="35"/>
+      <c r="B42" s="42"/>
+      <c r="C42" s="42"/>
+      <c r="D42" s="42"/>
+      <c r="E42" s="42"/>
+      <c r="F42" s="42"/>
+      <c r="G42" s="43"/>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
@@ -2111,20 +2126,40 @@
       <c r="F45" s="5"/>
       <c r="G45" s="6"/>
     </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="N46" t="s">
+        <v>103</v>
+      </c>
+      <c r="O46" t="s">
+        <v>0</v>
+      </c>
+      <c r="P46" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>105</v>
+      </c>
+      <c r="R46" t="s">
+        <v>106</v>
+      </c>
+      <c r="S46" t="s">
+        <v>107</v>
+      </c>
+    </row>
     <row r="48" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="49" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="22" t="s">
+      <c r="A49" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="B49" s="23"/>
-      <c r="C49" s="23"/>
-      <c r="D49" s="23"/>
-      <c r="E49" s="23"/>
-      <c r="F49" s="23"/>
-      <c r="G49" s="23"/>
-      <c r="H49" s="23"/>
-      <c r="I49" s="23"/>
-      <c r="J49" s="24"/>
+      <c r="B49" s="37"/>
+      <c r="C49" s="37"/>
+      <c r="D49" s="37"/>
+      <c r="E49" s="37"/>
+      <c r="F49" s="37"/>
+      <c r="G49" s="37"/>
+      <c r="H49" s="37"/>
+      <c r="I49" s="37"/>
+      <c r="J49" s="38"/>
       <c r="K49" s="18"/>
       <c r="L49" s="18"/>
     </row>
@@ -2186,17 +2221,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="A20:G20"/>
-    <mergeCell ref="A14:L14"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="S14:T14"/>
-    <mergeCell ref="A2:O2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="L20:T20"/>
-    <mergeCell ref="A36:H36"/>
-    <mergeCell ref="A30:E30"/>
     <mergeCell ref="A49:J49"/>
     <mergeCell ref="Y7:Z7"/>
     <mergeCell ref="M7:N7"/>
@@ -2211,6 +2235,17 @@
     <mergeCell ref="A42:G42"/>
     <mergeCell ref="L30:O30"/>
     <mergeCell ref="L25:T25"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="A20:G20"/>
+    <mergeCell ref="A14:L14"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="S14:T14"/>
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="L20:T20"/>
+    <mergeCell ref="A36:H36"/>
+    <mergeCell ref="A30:E30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
the error with the student_fee_routes; running_fee+running_dicount corrected
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10125"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10201"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ibrahim/Documents/python_project/db_system/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E70DEF69-9986-F543-A31E-5B428D01C22E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E347F7-9136-FF4C-97F4-509AC8BFD6DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15640" xr2:uid="{519AA96D-D64B-C848-85D8-98116B17AEBE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27600" windowHeight="15640" xr2:uid="{519AA96D-D64B-C848-85D8-98116B17AEBE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -836,7 +836,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -856,6 +856,69 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -865,18 +928,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -896,60 +947,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1286,10 +1283,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8650A0-ED64-5B4B-A401-C81B8C806AFE}">
-  <dimension ref="A1:Z62"/>
+  <dimension ref="A1:Z60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M35" workbookViewId="0">
-      <selection activeCell="R44" sqref="R44"/>
+    <sheetView tabSelected="1" topLeftCell="J40" workbookViewId="0">
+      <selection activeCell="V67" sqref="V67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1320,35 +1317,35 @@
   <sheetData>
     <row r="1" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="25"/>
-      <c r="Q2" s="24" t="s">
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="39"/>
+      <c r="Q2" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="R2" s="25"/>
-      <c r="T2" s="38" t="s">
+      <c r="R2" s="39"/>
+      <c r="T2" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="U2" s="39"/>
-      <c r="W2" s="38" t="s">
+      <c r="U2" s="35"/>
+      <c r="W2" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="X2" s="39"/>
+      <c r="X2" s="35"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
@@ -1487,40 +1484,40 @@
     </row>
     <row r="6" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="23"/>
-      <c r="J7" s="24" t="s">
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="33"/>
+      <c r="J7" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="K7" s="25"/>
-      <c r="M7" s="22" t="s">
+      <c r="K7" s="39"/>
+      <c r="M7" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="N7" s="23"/>
-      <c r="P7" s="26" t="s">
+      <c r="N7" s="33"/>
+      <c r="P7" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="Q7" s="27"/>
-      <c r="S7" s="22" t="s">
+      <c r="Q7" s="44"/>
+      <c r="S7" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="T7" s="23"/>
-      <c r="V7" s="22" t="s">
+      <c r="T7" s="33"/>
+      <c r="V7" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="W7" s="23"/>
-      <c r="Y7" s="22" t="s">
+      <c r="W7" s="33"/>
+      <c r="Y7" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="Z7" s="23"/>
+      <c r="Z7" s="33"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
@@ -1700,25 +1697,25 @@
     </row>
     <row r="13" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="B14" s="33"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="33"/>
-      <c r="K14" s="33"/>
-      <c r="L14" s="23"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="32"/>
+      <c r="L14" s="33"/>
       <c r="M14" s="18"/>
       <c r="N14" s="18"/>
       <c r="O14" s="18"/>
-      <c r="S14" s="40"/>
-      <c r="T14" s="40"/>
+      <c r="S14" s="36"/>
+      <c r="T14" s="36"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
@@ -1788,26 +1785,26 @@
     </row>
     <row r="19" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="24" t="s">
+      <c r="A20" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="25"/>
-      <c r="L20" s="34" t="s">
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="39"/>
+      <c r="L20" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="M20" s="35"/>
-      <c r="N20" s="35"/>
-      <c r="O20" s="35"/>
-      <c r="P20" s="35"/>
-      <c r="Q20" s="35"/>
-      <c r="R20" s="35"/>
-      <c r="S20" s="35"/>
-      <c r="T20" s="36"/>
+      <c r="M20" s="25"/>
+      <c r="N20" s="25"/>
+      <c r="O20" s="25"/>
+      <c r="P20" s="25"/>
+      <c r="Q20" s="25"/>
+      <c r="R20" s="25"/>
+      <c r="S20" s="25"/>
+      <c r="T20" s="26"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
@@ -1897,27 +1894,27 @@
     </row>
     <row r="24" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L25" s="34" t="s">
+      <c r="L25" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="M25" s="35"/>
-      <c r="N25" s="35"/>
-      <c r="O25" s="35"/>
-      <c r="P25" s="35"/>
-      <c r="Q25" s="35"/>
-      <c r="R25" s="35"/>
-      <c r="S25" s="35"/>
-      <c r="T25" s="36"/>
+      <c r="M25" s="25"/>
+      <c r="N25" s="25"/>
+      <c r="O25" s="25"/>
+      <c r="P25" s="25"/>
+      <c r="Q25" s="25"/>
+      <c r="R25" s="25"/>
+      <c r="S25" s="25"/>
+      <c r="T25" s="26"/>
     </row>
     <row r="26" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="30" t="s">
+      <c r="A26" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="31"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="32"/>
+      <c r="B26" s="48"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="48"/>
+      <c r="E26" s="48"/>
+      <c r="F26" s="49"/>
       <c r="L26" s="10" t="s">
         <v>67</v>
       </c>
@@ -1987,19 +1984,19 @@
       <c r="T28" s="6"/>
     </row>
     <row r="29" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I29" s="28" t="s">
+      <c r="I29" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="J29" s="29"/>
+      <c r="J29" s="46"/>
     </row>
     <row r="30" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="41" t="s">
+      <c r="A30" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="B30" s="42"/>
-      <c r="C30" s="42"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="43"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="29"/>
       <c r="F30" s="18"/>
       <c r="G30" s="18"/>
       <c r="I30" s="10" t="s">
@@ -2008,19 +2005,19 @@
       <c r="J30" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="L30" s="34" t="s">
+      <c r="L30" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="M30" s="35"/>
-      <c r="N30" s="35"/>
-      <c r="O30" s="36"/>
+      <c r="M30" s="25"/>
+      <c r="N30" s="25"/>
+      <c r="O30" s="26"/>
       <c r="P30" s="18"/>
-      <c r="Q30" s="34" t="s">
+      <c r="Q30" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="R30" s="35"/>
-      <c r="S30" s="35"/>
-      <c r="T30" s="36"/>
+      <c r="R30" s="25"/>
+      <c r="S30" s="25"/>
+      <c r="T30" s="26"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
@@ -2107,16 +2104,16 @@
     </row>
     <row r="35" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="41" t="s">
+      <c r="A36" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="42"/>
-      <c r="C36" s="42"/>
-      <c r="D36" s="42"/>
-      <c r="E36" s="42"/>
-      <c r="F36" s="42"/>
-      <c r="G36" s="42"/>
-      <c r="H36" s="43"/>
+      <c r="B36" s="28"/>
+      <c r="C36" s="28"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="28"/>
+      <c r="H36" s="29"/>
       <c r="I36" s="18"/>
       <c r="J36" s="18"/>
       <c r="K36" s="18"/>
@@ -2148,10 +2145,10 @@
       <c r="H37" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="J37" s="28" t="s">
+      <c r="J37" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="K37" s="29"/>
+      <c r="K37" s="46"/>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
@@ -2190,15 +2187,15 @@
     </row>
     <row r="41" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="42" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="B42" s="31"/>
-      <c r="C42" s="31"/>
-      <c r="D42" s="31"/>
-      <c r="E42" s="31"/>
-      <c r="F42" s="31"/>
-      <c r="G42" s="32"/>
+      <c r="B42" s="48"/>
+      <c r="C42" s="48"/>
+      <c r="D42" s="48"/>
+      <c r="E42" s="48"/>
+      <c r="F42" s="48"/>
+      <c r="G42" s="49"/>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
@@ -2240,19 +2237,19 @@
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
       <c r="G45" s="6"/>
-      <c r="N45" s="50" t="s">
+      <c r="N45" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="O45" s="51"/>
-      <c r="P45" s="51"/>
-      <c r="Q45" s="51"/>
-      <c r="R45" s="51"/>
-      <c r="S45" s="51"/>
-      <c r="T45" s="52"/>
-      <c r="V45" s="50" t="s">
+      <c r="O45" s="30"/>
+      <c r="P45" s="30"/>
+      <c r="Q45" s="30"/>
+      <c r="R45" s="30"/>
+      <c r="S45" s="30"/>
+      <c r="T45" s="23"/>
+      <c r="V45" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="W45" s="52"/>
+      <c r="W45" s="23"/>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.2">
       <c r="N46" s="10" t="s">
@@ -2313,23 +2310,23 @@
         <v>131</v>
       </c>
     </row>
-    <row r="49" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="19" t="s">
+    <row r="49" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="B49" s="20"/>
-      <c r="C49" s="20"/>
-      <c r="D49" s="20"/>
-      <c r="E49" s="20"/>
-      <c r="F49" s="20"/>
-      <c r="G49" s="20"/>
-      <c r="H49" s="20"/>
-      <c r="I49" s="20"/>
-      <c r="J49" s="21"/>
+      <c r="B49" s="41"/>
+      <c r="C49" s="41"/>
+      <c r="D49" s="41"/>
+      <c r="E49" s="41"/>
+      <c r="F49" s="41"/>
+      <c r="G49" s="41"/>
+      <c r="H49" s="41"/>
+      <c r="I49" s="41"/>
+      <c r="J49" s="42"/>
       <c r="K49" s="18"/>
       <c r="L49" s="18"/>
     </row>
-    <row r="50" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
         <v>71</v>
       </c>
@@ -2361,7 +2358,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="51" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -2372,21 +2369,21 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
       <c r="J51" s="3"/>
-      <c r="N51" s="47" t="s">
+      <c r="N51" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="O51" s="48"/>
-      <c r="P51" s="48"/>
-      <c r="Q51" s="48"/>
-      <c r="R51" s="48"/>
-      <c r="S51" s="48"/>
-      <c r="T51" s="48"/>
-      <c r="U51" s="48"/>
-      <c r="V51" s="48"/>
-      <c r="W51" s="48"/>
-      <c r="X51" s="49"/>
-    </row>
-    <row r="52" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="O51" s="20"/>
+      <c r="P51" s="20"/>
+      <c r="Q51" s="20"/>
+      <c r="R51" s="20"/>
+      <c r="S51" s="20"/>
+      <c r="T51" s="20"/>
+      <c r="U51" s="20"/>
+      <c r="V51" s="20"/>
+      <c r="W51" s="20"/>
+      <c r="X51" s="21"/>
+    </row>
+    <row r="52" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
@@ -2427,11 +2424,11 @@
       <c r="W52" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="X52" s="44" t="s">
+      <c r="X52" s="11" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.2">
       <c r="N53" s="2"/>
       <c r="O53" s="1"/>
       <c r="P53" s="1"/>
@@ -2444,7 +2441,7 @@
       <c r="W53" s="1"/>
       <c r="X53" s="3"/>
     </row>
-    <row r="54" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="N54" s="4"/>
       <c r="O54" s="5"/>
       <c r="P54" s="5"/>
@@ -2457,19 +2454,25 @@
       <c r="W54" s="5"/>
       <c r="X54" s="6"/>
     </row>
-    <row r="56" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="N57" s="47" t="s">
+    <row r="56" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="N57" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="O57" s="48"/>
-      <c r="P57" s="48"/>
-      <c r="Q57" s="48"/>
-      <c r="R57" s="48"/>
-      <c r="S57" s="49"/>
-      <c r="T57" s="46"/>
-    </row>
-    <row r="58" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="O57" s="20"/>
+      <c r="P57" s="20"/>
+      <c r="Q57" s="20"/>
+      <c r="R57" s="20"/>
+      <c r="S57" s="21"/>
+      <c r="U57" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="V57" s="20"/>
+      <c r="W57" s="20"/>
+      <c r="X57" s="20"/>
+      <c r="Y57" s="21"/>
+    </row>
+    <row r="58" spans="1:25" x14ac:dyDescent="0.2">
       <c r="N58" s="8" t="s">
         <v>103</v>
       </c>
@@ -2488,77 +2491,77 @@
       <c r="S58" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="T58" s="45"/>
-    </row>
-    <row r="59" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U58" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="V58" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="W58" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="X58" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="Y58" s="11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="59" spans="1:25" x14ac:dyDescent="0.2">
       <c r="N59" s="1"/>
       <c r="O59" s="1"/>
       <c r="P59" s="1"/>
       <c r="Q59" s="1"/>
       <c r="R59" s="1"/>
       <c r="S59" s="1"/>
-      <c r="T59" s="45"/>
-      <c r="V59" s="47" t="s">
-        <v>134</v>
-      </c>
-      <c r="W59" s="48"/>
-      <c r="X59" s="48"/>
-      <c r="Y59" s="48"/>
-      <c r="Z59" s="49"/>
-    </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="U59" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="V59" s="1">
+        <v>20</v>
+      </c>
+      <c r="W59" s="1">
+        <v>20</v>
+      </c>
+      <c r="X59" s="1">
+        <v>30</v>
+      </c>
+      <c r="Y59" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="N60" s="1"/>
       <c r="O60" s="1"/>
       <c r="P60" s="1"/>
       <c r="Q60" s="1"/>
       <c r="R60" s="1"/>
       <c r="S60" s="1"/>
-      <c r="T60" s="45"/>
-      <c r="V60" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="W60" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="X60" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="Y60" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="Z60" s="11" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="V61" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="W61" s="1">
-        <v>20</v>
-      </c>
-      <c r="X61" s="1">
-        <v>20</v>
-      </c>
-      <c r="Y61" s="1">
-        <v>30</v>
-      </c>
-      <c r="Z61" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="62" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="V62" s="4" t="s">
+      <c r="U60" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="W62" s="5"/>
-      <c r="X62" s="5"/>
-      <c r="Y62" s="5"/>
-      <c r="Z62" s="6"/>
+      <c r="V60" s="5"/>
+      <c r="W60" s="5"/>
+      <c r="X60" s="5"/>
+      <c r="Y60" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="V59:Z59"/>
+    <mergeCell ref="A20:G20"/>
+    <mergeCell ref="Y7:Z7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="V7:W7"/>
+    <mergeCell ref="A14:L14"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="S14:T14"/>
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="U57:Y57"/>
     <mergeCell ref="V45:W45"/>
     <mergeCell ref="N57:S57"/>
     <mergeCell ref="L20:T20"/>
@@ -2566,28 +2569,14 @@
     <mergeCell ref="A30:E30"/>
     <mergeCell ref="N45:T45"/>
     <mergeCell ref="N51:X51"/>
-    <mergeCell ref="A14:L14"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="S14:T14"/>
-    <mergeCell ref="A2:O2"/>
-    <mergeCell ref="Q2:R2"/>
     <mergeCell ref="A49:J49"/>
-    <mergeCell ref="Y7:Z7"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="S7:T7"/>
     <mergeCell ref="I29:J29"/>
     <mergeCell ref="A26:F26"/>
-    <mergeCell ref="A7:H7"/>
-    <mergeCell ref="V7:W7"/>
     <mergeCell ref="Q30:T30"/>
     <mergeCell ref="A42:G42"/>
     <mergeCell ref="L30:O30"/>
     <mergeCell ref="L25:T25"/>
     <mergeCell ref="J37:K37"/>
-    <mergeCell ref="A20:G20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>